<commit_message>
chore: beautify write to file
</commit_message>
<xml_diff>
--- a/files/template_format.xlsx
+++ b/files/template_format.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lunba7th\Documents\S2 - Teknik Sipil\S2 Thesis start from 0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\lunba\Project\ga_civil_construction_resource_optimization\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13032"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22656" windowHeight="9540"/>
   </bookViews>
   <sheets>
     <sheet name="Template Format Utama" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="146">
   <si>
     <t>PEKERJAAN</t>
   </si>
@@ -427,18 +427,56 @@
   </si>
   <si>
     <t>III.6</t>
+  </si>
+  <si>
+    <t>ANALISIS II (GA)</t>
+  </si>
+  <si>
+    <t>HASIL/REKOMENDASI (GA)</t>
+  </si>
+  <si>
+    <t>Capaian 1 Hari Kerja (1 org)</t>
+  </si>
+  <si>
+    <t>Total Pekerja</t>
+  </si>
+  <si>
+    <t>Total Hari Pengerjaan</t>
+  </si>
+  <si>
+    <t>Total Biaya Pekerja</t>
+  </si>
+  <si>
+    <t>TOTAL PEKERJA</t>
+  </si>
+  <si>
+    <t>Orang</t>
+  </si>
+  <si>
+    <t>TOTAL HARI PENGERJAAN PROYEK (PEKERJA)</t>
+  </si>
+  <si>
+    <t>Hari</t>
+  </si>
+  <si>
+    <t>TOTAL BIAYA PEKERJA</t>
+  </si>
+  <si>
+    <t>(Rp)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$IDR]\ #,##0.00;[Red][$IDR]\ #,##0.00"/>
+    <numFmt numFmtId="168" formatCode="[$IDR]\ #,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -590,7 +628,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -650,30 +688,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -684,20 +722,20 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -712,12 +750,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -729,7 +767,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -742,7 +780,7 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -754,27 +792,54 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1061,33 +1126,43 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:N281"/>
+  <dimension ref="B1:X281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:X1048576"/>
+      <selection pane="bottomLeft" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="5.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="12" customWidth="1"/>
     <col min="8" max="8" width="6.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="27" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" style="53" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" style="53" customWidth="1"/>
+    <col min="13" max="13" width="17.21875" style="12" customWidth="1"/>
     <col min="14" max="14" width="6" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="6"/>
+    <col min="20" max="20" width="17.21875" style="93" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.88671875" style="1"/>
+    <col min="22" max="22" width="39.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.88671875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
       <c r="E1" s="3"/>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
@@ -1096,30 +1171,43 @@
       <c r="K1" s="7"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="77"/>
-      <c r="C2" s="79" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B2" s="89"/>
+      <c r="C2" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
       <c r="N2" s="19"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
+      <c r="O2" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="V2" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B3" s="90"/>
+      <c r="C3" s="88"/>
       <c r="D3" s="20" t="s">
         <v>2</v>
       </c>
@@ -1149,24 +1237,57 @@
         <v>5</v>
       </c>
       <c r="N3" s="18"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="S3" s="87"/>
+      <c r="T3" s="94" t="s">
+        <v>139</v>
+      </c>
+      <c r="V3" s="88"/>
+      <c r="W3" s="88"/>
+      <c r="X3" s="88"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="76" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="79"/>
+      <c r="V4" s="80" t="s">
+        <v>140</v>
+      </c>
+      <c r="W4" s="81"/>
+      <c r="X4" s="82" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O5" s="79"/>
+      <c r="V5" s="83" t="s">
+        <v>142</v>
+      </c>
+      <c r="W5" s="84"/>
+      <c r="X5" s="82" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1207,8 +1328,18 @@
         <f>'Template Format ANALISIS I'!F3</f>
         <v>82500</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O6" s="79"/>
+      <c r="P6" s="85"/>
+      <c r="R6" s="79"/>
+      <c r="V6" s="80" t="s">
+        <v>144</v>
+      </c>
+      <c r="W6" s="86"/>
+      <c r="X6" s="82" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="E7" s="14"/>
       <c r="F7" s="15"/>
       <c r="G7" s="16"/>
@@ -1233,7 +1364,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
@@ -1246,12 +1377,12 @@
         <v>8550</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="E9" s="14"/>
       <c r="F9" s="15"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>3</v>
       </c>
@@ -1293,7 +1424,7 @@
         <v>27500</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I11" s="27">
         <f>'Template Format ANALISIS I'!B10</f>
         <v>8.3000000000000001E-3</v>
@@ -1315,7 +1446,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
       <c r="K12" s="13" t="str">
         <f>'Template Format ANALISIS I'!D11</f>
         <v>B.U &amp; Kentungan (10%)</v>
@@ -1325,7 +1456,7 @@
         <v>2849.6000000000004</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>4</v>
       </c>
@@ -1367,7 +1498,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F15" s="15"/>
       <c r="G15" s="16"/>
       <c r="I15" s="27">
@@ -1391,7 +1522,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I16" s="27">
         <f>'Template Format ANALISIS I'!B17</f>
         <v>1.2</v>
@@ -7190,11 +7321,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="V2:X3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="I2:M2"/>
+    <mergeCell ref="O2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chore: update constants and file to analyze
</commit_message>
<xml_diff>
--- a/files/template_format.xlsx
+++ b/files/template_format.xlsx
@@ -1005,7 +1005,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1251,19 +1251,10 @@
     <xf numFmtId="4" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1378,6 +1369,19 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
@@ -1667,7 +1671,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1430" sqref="K1430"/>
+      <selection pane="bottomLeft" activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1690,11 +1694,11 @@
     <col min="16" max="16" width="8.88671875" style="1"/>
     <col min="17" max="17" width="18.88671875" style="1" customWidth="1"/>
     <col min="18" max="18" width="22.88671875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="1"/>
-    <col min="20" max="20" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="148"/>
+    <col min="20" max="20" width="17.77734375" style="151" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.88671875" style="1"/>
     <col min="22" max="22" width="41.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.88671875" style="1"/>
+    <col min="23" max="23" width="33.109375" style="1" customWidth="1"/>
     <col min="24" max="24" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1707,49 +1711,49 @@
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B2" s="146"/>
-      <c r="C2" s="145" t="s">
+      <c r="B2" s="143"/>
+      <c r="C2" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="148" t="s">
+      <c r="D2" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="148"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="149" t="s">
+      <c r="I2" s="146" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="148"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="145"/>
       <c r="N2" s="18"/>
-      <c r="O2" s="148" t="s">
+      <c r="O2" s="145" t="s">
         <v>154</v>
       </c>
-      <c r="P2" s="148"/>
-      <c r="Q2" s="148"/>
-      <c r="R2" s="148"/>
-      <c r="S2" s="148"/>
-      <c r="T2" s="148"/>
-      <c r="V2" s="145" t="s">
+      <c r="P2" s="145"/>
+      <c r="Q2" s="145"/>
+      <c r="R2" s="145"/>
+      <c r="S2" s="145"/>
+      <c r="T2" s="145"/>
+      <c r="V2" s="142" t="s">
         <v>155</v>
       </c>
-      <c r="W2" s="145"/>
-      <c r="X2" s="145"/>
+      <c r="W2" s="142"/>
+      <c r="X2" s="142"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B3" s="147"/>
-      <c r="C3" s="145"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="142"/>
       <c r="D3" s="19" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="109" t="s">
+      <c r="F3" s="106" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="30" t="s">
@@ -1759,7 +1763,7 @@
       <c r="I3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="119" t="s">
+      <c r="J3" s="116" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="21" t="s">
@@ -1786,9 +1790,9 @@
       <c r="T3" s="85" t="s">
         <v>159</v>
       </c>
-      <c r="V3" s="145"/>
-      <c r="W3" s="145"/>
-      <c r="X3" s="145"/>
+      <c r="V3" s="142"/>
+      <c r="W3" s="142"/>
+      <c r="X3" s="142"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" s="70" t="s">
@@ -1799,7 +1803,7 @@
       </c>
       <c r="D4" s="96"/>
       <c r="E4" s="97"/>
-      <c r="F4" s="110"/>
+      <c r="F4" s="107"/>
       <c r="G4" s="98"/>
       <c r="H4" s="32"/>
       <c r="I4" s="99"/>
@@ -1808,12 +1812,12 @@
       <c r="L4" s="101"/>
       <c r="M4" s="102"/>
       <c r="N4" s="17"/>
-      <c r="O4" s="103"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="105"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="107"/>
+      <c r="O4" s="147"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="104"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="150"/>
       <c r="V4" s="88" t="s">
         <v>160</v>
       </c>
@@ -1832,10 +1836,10 @@
       <c r="D5" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="108">
+      <c r="E5" s="105">
         <v>500</v>
       </c>
-      <c r="F5" s="113">
+      <c r="F5" s="110">
         <v>18000</v>
       </c>
       <c r="G5" s="15">
@@ -1843,7 +1847,7 @@
         <v>9000000</v>
       </c>
       <c r="H5" s="32"/>
-      <c r="I5" s="123">
+      <c r="I5" s="120">
         <v>0.5</v>
       </c>
       <c r="J5" s="38" t="s">
@@ -1852,17 +1856,17 @@
       <c r="K5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="113">
+      <c r="L5" s="110">
         <v>110000</v>
       </c>
       <c r="M5" s="102"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="105"/>
-      <c r="R5" s="105"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="107"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="104"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="150"/>
       <c r="V5" s="91" t="s">
         <v>162</v>
       </c>
@@ -1875,22 +1879,22 @@
       <c r="B6" s="7"/>
       <c r="C6" s="6"/>
       <c r="D6" s="34"/>
-      <c r="E6" s="108"/>
+      <c r="E6" s="105"/>
       <c r="F6" s="66"/>
       <c r="G6" s="15"/>
       <c r="H6" s="32"/>
-      <c r="I6" s="112"/>
+      <c r="I6" s="109"/>
       <c r="J6" s="38"/>
       <c r="K6" s="38"/>
       <c r="L6" s="80"/>
       <c r="M6" s="102"/>
       <c r="N6" s="17"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="104"/>
-      <c r="Q6" s="105"/>
-      <c r="R6" s="105"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="107"/>
+      <c r="O6" s="147"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="104"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="150"/>
       <c r="V6" s="88" t="s">
         <v>164</v>
       </c>
@@ -1909,10 +1913,10 @@
       <c r="D7" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="E7" s="108">
+      <c r="E7" s="105">
         <v>1</v>
       </c>
-      <c r="F7" s="113">
+      <c r="F7" s="110">
         <v>5000000</v>
       </c>
       <c r="G7" s="15">
@@ -1920,7 +1924,7 @@
         <v>5000000</v>
       </c>
       <c r="H7" s="32"/>
-      <c r="I7" s="123">
+      <c r="I7" s="120">
         <v>0.5</v>
       </c>
       <c r="J7" s="38" t="s">
@@ -1929,19 +1933,19 @@
       <c r="K7" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="113">
+      <c r="L7" s="110">
         <v>110000</v>
       </c>
       <c r="M7" s="102"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="103"/>
-      <c r="P7" s="104"/>
-      <c r="Q7" s="105"/>
-      <c r="R7" s="105"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="107"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="118"/>
+      <c r="O7" s="147"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="104"/>
+      <c r="R7" s="104"/>
+      <c r="S7" s="104"/>
+      <c r="T7" s="150"/>
+      <c r="V7" s="114"/>
+      <c r="W7" s="115"/>
       <c r="X7" s="7"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
@@ -1949,7 +1953,7 @@
       <c r="C8" s="95"/>
       <c r="D8" s="96"/>
       <c r="E8" s="97"/>
-      <c r="F8" s="110"/>
+      <c r="F8" s="107"/>
       <c r="G8" s="98"/>
       <c r="H8" s="32"/>
       <c r="I8" s="99"/>
@@ -1958,14 +1962,14 @@
       <c r="L8" s="80"/>
       <c r="M8" s="102"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="104"/>
-      <c r="Q8" s="105"/>
-      <c r="R8" s="105"/>
-      <c r="S8" s="106"/>
-      <c r="T8" s="107"/>
-      <c r="V8" s="117"/>
-      <c r="W8" s="118"/>
+      <c r="O8" s="147"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="104"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="104"/>
+      <c r="T8" s="150"/>
+      <c r="V8" s="114"/>
+      <c r="W8" s="115"/>
       <c r="X8" s="7"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -1979,10 +1983,10 @@
       <c r="O9" s="86"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
+      <c r="S9" s="149"/>
       <c r="T9" s="87"/>
-      <c r="V9" s="117"/>
-      <c r="W9" s="118"/>
+      <c r="V9" s="114"/>
+      <c r="W9" s="115"/>
       <c r="X9" s="7"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
@@ -1996,10 +2000,10 @@
       <c r="O10" s="86"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
+      <c r="S10" s="149"/>
       <c r="T10" s="87"/>
-      <c r="V10" s="117"/>
-      <c r="W10" s="118"/>
+      <c r="V10" s="114"/>
+      <c r="W10" s="115"/>
       <c r="X10" s="7"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
@@ -2015,14 +2019,14 @@
       <c r="E11" s="11">
         <v>262.08</v>
       </c>
-      <c r="F11" s="114">
+      <c r="F11" s="111">
         <v>41360</v>
       </c>
       <c r="G11" s="15">
         <f>E11*F11</f>
         <v>10839628.799999999</v>
       </c>
-      <c r="I11" s="116">
+      <c r="I11" s="113">
         <v>0.5</v>
       </c>
       <c r="J11" s="13" t="s">
@@ -2031,16 +2035,16 @@
       <c r="K11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="113">
+      <c r="L11" s="110">
         <v>110000</v>
       </c>
       <c r="O11" s="86"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
+      <c r="S11" s="149"/>
       <c r="T11" s="87"/>
-      <c r="V11" s="117"/>
-      <c r="W11" s="118"/>
+      <c r="V11" s="114"/>
+      <c r="W11" s="115"/>
       <c r="X11" s="7"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
@@ -2049,7 +2053,7 @@
       <c r="O12" s="86"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
+      <c r="S12" s="149"/>
       <c r="T12" s="87"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
@@ -2065,7 +2069,7 @@
       <c r="E13" s="11">
         <v>122.08</v>
       </c>
-      <c r="F13" s="115">
+      <c r="F13" s="112">
         <f>'Template Format ANALISIS I'!F255 - 31669</f>
         <v>136631</v>
       </c>
@@ -2096,7 +2100,7 @@
       <c r="O13" s="86"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
+      <c r="S13" s="149"/>
       <c r="T13" s="87"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
@@ -2124,7 +2128,7 @@
       <c r="O14" s="86"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
+      <c r="S14" s="149"/>
       <c r="T14" s="87"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
@@ -2142,7 +2146,7 @@
       <c r="O15" s="86"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
+      <c r="S15" s="149"/>
       <c r="T15" s="87"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.3">
@@ -2151,7 +2155,7 @@
       <c r="O16" s="86"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
+      <c r="S16" s="149"/>
       <c r="T16" s="87"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
@@ -2167,7 +2171,7 @@
       <c r="E17" s="14">
         <v>90</v>
       </c>
-      <c r="F17" s="111">
+      <c r="F17" s="108">
         <f>'Template Format ANALISIS I'!F6</f>
         <v>94050</v>
       </c>
@@ -2199,12 +2203,12 @@
       <c r="P17" s="93"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="86"/>
-      <c r="S17" s="6"/>
+      <c r="S17" s="149"/>
       <c r="T17" s="87"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E18" s="14"/>
-      <c r="F18" s="111"/>
+      <c r="F18" s="108"/>
       <c r="G18" s="15"/>
       <c r="I18" s="25">
         <f>'Template Format ANALISIS I'!B4</f>
@@ -2229,7 +2233,7 @@
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E19" s="14"/>
-      <c r="F19" s="111"/>
+      <c r="F19" s="108"/>
       <c r="G19" s="15"/>
       <c r="K19" s="13" t="str">
         <f>'Template Format ANALISIS I'!D5</f>
@@ -2242,7 +2246,7 @@
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E20" s="14"/>
-      <c r="F20" s="111"/>
+      <c r="F20" s="108"/>
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.3">
@@ -2258,7 +2262,7 @@
       <c r="E21" s="14">
         <v>40.69</v>
       </c>
-      <c r="F21" s="111">
+      <c r="F21" s="108">
         <f>'Template Format ANALISIS I'!F12</f>
         <v>31345.599999999999</v>
       </c>
@@ -2332,7 +2336,7 @@
       <c r="E25" s="11">
         <v>22</v>
       </c>
-      <c r="F25" s="111">
+      <c r="F25" s="108">
         <f>'Template Format ANALISIS I'!F19</f>
         <v>301620</v>
       </c>
@@ -2362,7 +2366,7 @@
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="F26" s="111"/>
+      <c r="F26" s="108"/>
       <c r="G26" s="15"/>
       <c r="I26" s="25">
         <f>'Template Format ANALISIS I'!B16</f>
@@ -2430,7 +2434,7 @@
       <c r="E30" s="11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F30" s="111">
+      <c r="F30" s="108">
         <f>'Template Format ANALISIS I'!F28</f>
         <v>583044</v>
       </c>
@@ -2594,7 +2598,7 @@
       <c r="E38" s="11">
         <v>72</v>
       </c>
-      <c r="F38" s="111">
+      <c r="F38" s="108">
         <f>'Template Format ANALISIS I'!F35</f>
         <v>158620</v>
       </c>
@@ -2624,7 +2628,7 @@
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F39" s="111"/>
+      <c r="F39" s="108"/>
       <c r="I39" s="39">
         <f>'Template Format ANALISIS I'!B32</f>
         <v>0.01</v>
@@ -2647,7 +2651,7 @@
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F40" s="111"/>
+      <c r="F40" s="108"/>
       <c r="I40" s="39">
         <f>'Template Format ANALISIS I'!B33</f>
         <v>1</v>
@@ -2708,7 +2712,7 @@
       <c r="E45" s="11">
         <v>122.08</v>
       </c>
-      <c r="F45" s="115">
+      <c r="F45" s="112">
         <f>'Template Format ANALISIS I'!F263 - 65505</f>
         <v>1619860</v>
       </c>
@@ -2720,11 +2724,11 @@
         <f>'Template Format ANALISIS I'!B258</f>
         <v>0.876</v>
       </c>
-      <c r="J45" s="118" t="str">
+      <c r="J45" s="115" t="str">
         <f>'Template Format ANALISIS I'!C258</f>
         <v>OH</v>
       </c>
-      <c r="K45" s="118" t="str">
+      <c r="K45" s="115" t="str">
         <f>'Template Format ANALISIS I'!D258</f>
         <v>Pekerja</v>
       </c>
@@ -2742,11 +2746,11 @@
         <f>'Template Format ANALISIS I'!B259</f>
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="J46" s="118" t="str">
+      <c r="J46" s="115" t="str">
         <f>'Template Format ANALISIS I'!C259</f>
         <v>OH</v>
       </c>
-      <c r="K46" s="118" t="str">
+      <c r="K46" s="115" t="str">
         <f>'Template Format ANALISIS I'!D259</f>
         <v>Mandor</v>
       </c>
@@ -2764,11 +2768,11 @@
         <f>'Template Format ANALISIS I'!B260</f>
         <v>1</v>
       </c>
-      <c r="J47" s="118" t="str">
+      <c r="J47" s="115" t="str">
         <f>'Template Format ANALISIS I'!C260</f>
         <v>M3</v>
       </c>
-      <c r="K47" s="118" t="str">
+      <c r="K47" s="115" t="str">
         <f>'Template Format ANALISIS I'!D260</f>
         <v>Beton Ready Mix K-300</v>
       </c>
@@ -2788,11 +2792,11 @@
         <f>'Template Format ANALISIS I'!B261</f>
         <v>0.5</v>
       </c>
-      <c r="J48" s="118" t="str">
+      <c r="J48" s="115" t="str">
         <f>'Template Format ANALISIS I'!C261</f>
         <v>Jam</v>
       </c>
-      <c r="K48" s="118" t="str">
+      <c r="K48" s="115" t="str">
         <f>'Template Format ANALISIS I'!D261</f>
         <v>Concrete Pump</v>
       </c>
@@ -2809,8 +2813,8 @@
       <c r="B49" s="71"/>
       <c r="C49" s="10"/>
       <c r="I49" s="26"/>
-      <c r="J49" s="118"/>
-      <c r="K49" s="118" t="str">
+      <c r="J49" s="115"/>
+      <c r="K49" s="115" t="str">
         <f>'Template Format ANALISIS I'!D262</f>
         <v>B.U &amp; Kentungan (10%)</v>
       </c>
@@ -2837,7 +2841,7 @@
       <c r="E51" s="11">
         <v>13337.71</v>
       </c>
-      <c r="F51" s="115">
+      <c r="F51" s="112">
         <f>'Template Format ANALISIS I'!F275 - 538.5</f>
         <v>20000</v>
       </c>
@@ -2849,11 +2853,11 @@
         <f>'Template Format ANALISIS I'!B268</f>
         <v>7.000000000000001E-3</v>
       </c>
-      <c r="J51" s="118" t="str">
+      <c r="J51" s="115" t="str">
         <f>'Template Format ANALISIS I'!C268</f>
         <v>OH</v>
       </c>
-      <c r="K51" s="118" t="str">
+      <c r="K51" s="115" t="str">
         <f>'Template Format ANALISIS I'!D268</f>
         <v xml:space="preserve">Pekerja </v>
       </c>
@@ -2873,11 +2877,11 @@
         <f>'Template Format ANALISIS I'!B269</f>
         <v>7.000000000000001E-3</v>
       </c>
-      <c r="J52" s="118" t="str">
+      <c r="J52" s="115" t="str">
         <f>'Template Format ANALISIS I'!C269</f>
         <v>OH</v>
       </c>
-      <c r="K52" s="118" t="str">
+      <c r="K52" s="115" t="str">
         <f>'Template Format ANALISIS I'!D269</f>
         <v>Tukang Besi</v>
       </c>
@@ -2897,11 +2901,11 @@
         <f>'Template Format ANALISIS I'!B270</f>
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="J53" s="118" t="str">
+      <c r="J53" s="115" t="str">
         <f>'Template Format ANALISIS I'!C270</f>
         <v>OH</v>
       </c>
-      <c r="K53" s="118" t="str">
+      <c r="K53" s="115" t="str">
         <f>'Template Format ANALISIS I'!D270</f>
         <v>Kepala Tukang</v>
       </c>
@@ -2921,11 +2925,11 @@
         <f>'Template Format ANALISIS I'!B271</f>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="J54" s="118" t="str">
+      <c r="J54" s="115" t="str">
         <f>'Template Format ANALISIS I'!C271</f>
         <v>OH</v>
       </c>
-      <c r="K54" s="118" t="str">
+      <c r="K54" s="115" t="str">
         <f>'Template Format ANALISIS I'!D271</f>
         <v>Mandor</v>
       </c>
@@ -2945,11 +2949,11 @@
         <f>'Template Format ANALISIS I'!B273</f>
         <v>1.05</v>
       </c>
-      <c r="J55" s="118" t="str">
+      <c r="J55" s="115" t="str">
         <f>'Template Format ANALISIS I'!C273</f>
         <v>Kg</v>
       </c>
-      <c r="K55" s="118" t="str">
+      <c r="K55" s="115" t="str">
         <f>'Template Format ANALISIS I'!D273</f>
         <v>Besi Beton Polos</v>
       </c>
@@ -2969,11 +2973,11 @@
         <f>'Template Format ANALISIS I'!B274</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J56" s="118" t="str">
+      <c r="J56" s="115" t="str">
         <f>'Template Format ANALISIS I'!C274</f>
         <v>Kg</v>
       </c>
-      <c r="K56" s="118" t="str">
+      <c r="K56" s="115" t="str">
         <f>'Template Format ANALISIS I'!D274</f>
         <v>Kawat Beton</v>
       </c>
@@ -2990,8 +2994,8 @@
       <c r="B57" s="71"/>
       <c r="C57" s="10"/>
       <c r="I57" s="26"/>
-      <c r="J57" s="118"/>
-      <c r="K57" s="118"/>
+      <c r="J57" s="115"/>
+      <c r="K57" s="115"/>
       <c r="L57" s="74"/>
       <c r="M57" s="44"/>
     </row>
@@ -3008,7 +3012,7 @@
       <c r="E58" s="11">
         <v>25.43</v>
       </c>
-      <c r="F58" s="115">
+      <c r="F58" s="112">
         <f>'Template Format ANALISIS I'!F289 - 31016</f>
         <v>270919</v>
       </c>
@@ -3020,11 +3024,11 @@
         <f>'Template Format ANALISIS I'!B280</f>
         <v>0.22</v>
       </c>
-      <c r="J58" s="118" t="str">
+      <c r="J58" s="115" t="str">
         <f>'Template Format ANALISIS I'!C280</f>
         <v>OH</v>
       </c>
-      <c r="K58" s="118" t="str">
+      <c r="K58" s="115" t="str">
         <f>'Template Format ANALISIS I'!D280</f>
         <v xml:space="preserve">Pekerja </v>
       </c>
@@ -3042,11 +3046,11 @@
         <f>'Template Format ANALISIS I'!B281</f>
         <v>1.1000000000000001E-2</v>
       </c>
-      <c r="J59" s="118" t="str">
+      <c r="J59" s="115" t="str">
         <f>'Template Format ANALISIS I'!C281</f>
         <v>OH</v>
       </c>
-      <c r="K59" s="118" t="str">
+      <c r="K59" s="115" t="str">
         <f>'Template Format ANALISIS I'!D281</f>
         <v>Mandor</v>
       </c>
@@ -3064,11 +3068,11 @@
         <f>'Template Format ANALISIS I'!B282</f>
         <v>0.16500000000000001</v>
       </c>
-      <c r="J60" s="118" t="str">
+      <c r="J60" s="115" t="str">
         <f>'Template Format ANALISIS I'!C282</f>
         <v>OH</v>
       </c>
-      <c r="K60" s="118" t="str">
+      <c r="K60" s="115" t="str">
         <f>'Template Format ANALISIS I'!D282</f>
         <v>Tukang Kayu</v>
       </c>
@@ -3086,11 +3090,11 @@
         <f>'Template Format ANALISIS I'!B283</f>
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="J61" s="118" t="str">
+      <c r="J61" s="115" t="str">
         <f>'Template Format ANALISIS I'!C283</f>
         <v>OH</v>
       </c>
-      <c r="K61" s="118" t="str">
+      <c r="K61" s="115" t="str">
         <f>'Template Format ANALISIS I'!D283</f>
         <v>Kepala Tukang</v>
       </c>
@@ -3108,11 +3112,11 @@
         <f>'Template Format ANALISIS I'!B285</f>
         <v>0.04</v>
       </c>
-      <c r="J62" s="118" t="str">
+      <c r="J62" s="115" t="str">
         <f>'Template Format ANALISIS I'!C285</f>
         <v>M3</v>
       </c>
-      <c r="K62" s="118" t="str">
+      <c r="K62" s="115" t="str">
         <f>'Template Format ANALISIS I'!D285</f>
         <v>Kayu Balok Kls III</v>
       </c>
@@ -3130,11 +3134,11 @@
         <f>'Template Format ANALISIS I'!B286</f>
         <v>0.3</v>
       </c>
-      <c r="J63" s="118" t="str">
+      <c r="J63" s="115" t="str">
         <f>'Template Format ANALISIS I'!C286</f>
         <v>Kg</v>
       </c>
-      <c r="K63" s="118" t="str">
+      <c r="K63" s="115" t="str">
         <f>'Template Format ANALISIS I'!D286</f>
         <v>Paku 5 cm - 12 cm</v>
       </c>
@@ -3152,11 +3156,11 @@
         <f>'Template Format ANALISIS I'!B287</f>
         <v>0.1</v>
       </c>
-      <c r="J64" s="118" t="str">
+      <c r="J64" s="115" t="str">
         <f>'Template Format ANALISIS I'!C287</f>
         <v>Ltr</v>
       </c>
-      <c r="K64" s="118" t="str">
+      <c r="K64" s="115" t="str">
         <f>'Template Format ANALISIS I'!D287</f>
         <v xml:space="preserve">Minyak Bekisting </v>
       </c>
@@ -3174,11 +3178,11 @@
         <f>'Template Format ANALISIS I'!B288</f>
         <v>0.82</v>
       </c>
-      <c r="J65" s="118" t="str">
+      <c r="J65" s="115" t="str">
         <f>'Template Format ANALISIS I'!C288</f>
         <v>Lbr</v>
       </c>
-      <c r="K65" s="118" t="str">
+      <c r="K65" s="115" t="str">
         <f>'Template Format ANALISIS I'!D288</f>
         <v>Plywood Tebal 9 mm/Papan</v>
       </c>
@@ -3195,8 +3199,8 @@
       <c r="B66" s="71"/>
       <c r="C66" s="10"/>
       <c r="I66" s="26"/>
-      <c r="J66" s="118"/>
-      <c r="K66" s="118"/>
+      <c r="J66" s="115"/>
+      <c r="K66" s="115"/>
       <c r="L66" s="74"/>
       <c r="M66" s="44"/>
     </row>
@@ -3208,8 +3212,8 @@
         <v>199</v>
       </c>
       <c r="I67" s="26"/>
-      <c r="J67" s="118"/>
-      <c r="K67" s="118"/>
+      <c r="J67" s="115"/>
+      <c r="K67" s="115"/>
       <c r="L67" s="74"/>
       <c r="M67" s="44"/>
     </row>
@@ -3226,7 +3230,7 @@
       <c r="E68" s="11">
         <v>42.24</v>
       </c>
-      <c r="F68" s="115">
+      <c r="F68" s="112">
         <f>'Template Format ANALISIS I'!F263 - 65505</f>
         <v>1619860</v>
       </c>
@@ -3355,7 +3359,7 @@
       <c r="E74" s="11">
         <v>4721.66</v>
       </c>
-      <c r="F74" s="115">
+      <c r="F74" s="112">
         <f>'Template Format ANALISIS I'!F275 - 538.5</f>
         <v>20000</v>
       </c>
@@ -3508,8 +3512,8 @@
       <c r="B80" s="71"/>
       <c r="C80" s="10"/>
       <c r="I80" s="26"/>
-      <c r="J80" s="118"/>
-      <c r="K80" s="118"/>
+      <c r="J80" s="115"/>
+      <c r="K80" s="115"/>
       <c r="L80" s="74"/>
       <c r="M80" s="44"/>
     </row>
@@ -3526,7 +3530,7 @@
       <c r="E81" s="11">
         <v>110.08</v>
       </c>
-      <c r="F81" s="115">
+      <c r="F81" s="112">
         <f>'Template Format ANALISIS I'!F289 - 31016</f>
         <v>270919</v>
       </c>
@@ -3726,7 +3730,7 @@
       <c r="E90" s="11">
         <v>84</v>
       </c>
-      <c r="F90" s="111">
+      <c r="F90" s="108">
         <f>'Template Format ANALISIS I'!F46</f>
         <v>990990</v>
       </c>
@@ -3923,7 +3927,7 @@
       <c r="E99" s="11">
         <v>18.989999999999998</v>
       </c>
-      <c r="F99" s="115">
+      <c r="F99" s="112">
         <f>'Template Format ANALISIS I'!F263 - 65505</f>
         <v>1619860</v>
       </c>
@@ -4054,7 +4058,7 @@
       <c r="E105" s="11">
         <v>4213.6000000000004</v>
       </c>
-      <c r="F105" s="115">
+      <c r="F105" s="112">
         <f>'Template Format ANALISIS I'!F275 - 538.5</f>
         <v>20000</v>
       </c>
@@ -4426,7 +4430,7 @@
       <c r="E122" s="11">
         <v>1.28</v>
       </c>
-      <c r="F122" s="115">
+      <c r="F122" s="112">
         <f>'Template Format ANALISIS I'!F263 - 65505</f>
         <v>1619860</v>
       </c>
@@ -4559,7 +4563,7 @@
       <c r="E128" s="11">
         <v>479.6</v>
       </c>
-      <c r="F128" s="115">
+      <c r="F128" s="112">
         <f>'Template Format ANALISIS I'!F275 - 538.5</f>
         <v>20000</v>
       </c>
@@ -4931,7 +4935,7 @@
       <c r="E144" s="11">
         <v>9.6</v>
       </c>
-      <c r="F144" s="115">
+      <c r="F144" s="112">
         <f>'Template Format ANALISIS I'!F263 - 65505</f>
         <v>1619860</v>
       </c>
@@ -5060,7 +5064,7 @@
       <c r="E150" s="11">
         <v>3762.33</v>
       </c>
-      <c r="F150" s="115">
+      <c r="F150" s="112">
         <f>'Template Format ANALISIS I'!F275 - 538.5</f>
         <v>20000</v>
       </c>
@@ -5217,7 +5221,7 @@
       <c r="E157" s="11">
         <v>108.8</v>
       </c>
-      <c r="F157" s="115">
+      <c r="F157" s="112">
         <f>'Template Format ANALISIS I'!F289 - 31016</f>
         <v>270919</v>
       </c>
@@ -5433,7 +5437,7 @@
       <c r="E167" s="11">
         <v>0.95</v>
       </c>
-      <c r="F167" s="115">
+      <c r="F167" s="112">
         <f>'Template Format ANALISIS I'!F263 - 65505</f>
         <v>1619860</v>
       </c>
@@ -5561,7 +5565,7 @@
       <c r="E173" s="11">
         <v>167.18</v>
       </c>
-      <c r="F173" s="115">
+      <c r="F173" s="112">
         <f>'Template Format ANALISIS I'!F275 - 538.5</f>
         <v>20000</v>
       </c>
@@ -5720,7 +5724,7 @@
       <c r="E180" s="11">
         <v>15.2</v>
       </c>
-      <c r="F180" s="115">
+      <c r="F180" s="112">
         <f>'Template Format ANALISIS I'!F289 - 31016</f>
         <v>270919</v>
       </c>
@@ -5750,7 +5754,7 @@
       </c>
     </row>
     <row r="181" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F181" s="118"/>
+      <c r="F181" s="115"/>
       <c r="I181" s="26">
         <f>'Template Format ANALISIS I'!B281</f>
         <v>1.1000000000000001E-2</v>
@@ -5773,7 +5777,7 @@
       </c>
     </row>
     <row r="182" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F182" s="118"/>
+      <c r="F182" s="115"/>
       <c r="I182" s="26">
         <f>'Template Format ANALISIS I'!B282</f>
         <v>0.16500000000000001</v>
@@ -5796,7 +5800,7 @@
       </c>
     </row>
     <row r="183" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F183" s="118"/>
+      <c r="F183" s="115"/>
       <c r="I183" s="26">
         <f>'Template Format ANALISIS I'!B283</f>
         <v>8.2500000000000004E-3</v>
@@ -5819,7 +5823,7 @@
       </c>
     </row>
     <row r="184" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F184" s="118"/>
+      <c r="F184" s="115"/>
       <c r="I184" s="26">
         <f>'Template Format ANALISIS I'!B285</f>
         <v>0.04</v>
@@ -5842,7 +5846,7 @@
       </c>
     </row>
     <row r="185" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F185" s="118"/>
+      <c r="F185" s="115"/>
       <c r="I185" s="26">
         <f>'Template Format ANALISIS I'!B286</f>
         <v>0.3</v>
@@ -5865,7 +5869,7 @@
       </c>
     </row>
     <row r="186" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F186" s="118"/>
+      <c r="F186" s="115"/>
       <c r="I186" s="26">
         <f>'Template Format ANALISIS I'!B287</f>
         <v>0.1</v>
@@ -5888,7 +5892,7 @@
       </c>
     </row>
     <row r="187" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F187" s="118"/>
+      <c r="F187" s="115"/>
       <c r="I187" s="26">
         <f>'Template Format ANALISIS I'!B288</f>
         <v>0.82</v>
@@ -5941,7 +5945,7 @@
       <c r="E190" s="11">
         <v>15.53</v>
       </c>
-      <c r="F190" s="115">
+      <c r="F190" s="112">
         <f>'Template Format ANALISIS I'!F263 - 65505</f>
         <v>1619860</v>
       </c>
@@ -6077,7 +6081,7 @@
       <c r="E196" s="11">
         <v>4357.4399999999996</v>
       </c>
-      <c r="F196" s="115">
+      <c r="F196" s="112">
         <f>'Template Format ANALISIS I'!F275 - 538.5</f>
         <v>20000</v>
       </c>
@@ -6469,7 +6473,7 @@
       <c r="E213" s="11">
         <v>74.8</v>
       </c>
-      <c r="F213" s="114">
+      <c r="F213" s="111">
         <f>'Template Format ANALISIS I'!F306 - 29795.75</f>
         <v>119818</v>
       </c>
@@ -6800,7 +6804,7 @@
       <c r="E228" s="11">
         <v>93.78</v>
       </c>
-      <c r="F228" s="114">
+      <c r="F228" s="111">
         <f>'Template Format ANALISIS I'!F323 - 642.5</f>
         <v>149084</v>
       </c>
@@ -7130,7 +7134,7 @@
       <c r="E244" s="11">
         <v>6.81</v>
       </c>
-      <c r="F244" s="111">
+      <c r="F244" s="108">
         <f>'Template Format ANALISIS I'!F19</f>
         <v>301620</v>
       </c>
@@ -7226,14 +7230,14 @@
       <c r="E249" s="11">
         <v>68.099999999999994</v>
       </c>
-      <c r="F249" s="114">
+      <c r="F249" s="111">
         <v>110000</v>
       </c>
       <c r="G249" s="12">
         <f>F249*E249</f>
         <v>7490999.9999999991</v>
       </c>
-      <c r="I249" s="116">
+      <c r="I249" s="113">
         <v>0.5</v>
       </c>
       <c r="J249" s="13" t="s">
@@ -7242,7 +7246,7 @@
       <c r="K249" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L249" s="124">
+      <c r="L249" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -7267,7 +7271,7 @@
       <c r="E252" s="11">
         <v>12</v>
       </c>
-      <c r="F252" s="111">
+      <c r="F252" s="108">
         <f>'Template Format ANALISIS I'!F19</f>
         <v>301620</v>
       </c>
@@ -7639,7 +7643,7 @@
       <c r="E267" s="35">
         <v>219.6</v>
       </c>
-      <c r="F267" s="113">
+      <c r="F267" s="110">
         <f>'Template Format ANALISIS I'!F334 - 291381</f>
         <v>293104</v>
       </c>
@@ -7890,7 +7894,7 @@
       <c r="E276" s="35">
         <v>9.68</v>
       </c>
-      <c r="F276" s="113">
+      <c r="F276" s="110">
         <f>'Template Format ANALISIS I'!F345 - 66973</f>
         <v>249057</v>
       </c>
@@ -8130,10 +8134,10 @@
       <c r="E285" s="11">
         <v>15.6</v>
       </c>
-      <c r="F285" s="114">
+      <c r="F285" s="111">
         <v>120000</v>
       </c>
-      <c r="I285" s="125">
+      <c r="I285" s="122">
         <v>5</v>
       </c>
       <c r="J285" s="13" t="s">
@@ -8142,7 +8146,7 @@
       <c r="K285" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L285" s="124">
+      <c r="L285" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -8390,7 +8394,7 @@
       <c r="E296" s="35">
         <v>14</v>
       </c>
-      <c r="F296" s="113">
+      <c r="F296" s="110">
         <f>'Template Format ANALISIS I'!F355 - 26939</f>
         <v>43857</v>
       </c>
@@ -8399,7 +8403,7 @@
         <v>613998</v>
       </c>
       <c r="H296" s="32"/>
-      <c r="I296" s="134">
+      <c r="I296" s="131">
         <f>'Template Format ANALISIS I'!B348</f>
         <v>0.12</v>
       </c>
@@ -8428,7 +8432,7 @@
       <c r="F297" s="80"/>
       <c r="G297" s="36"/>
       <c r="H297" s="32"/>
-      <c r="I297" s="134">
+      <c r="I297" s="131">
         <f>'Template Format ANALISIS I'!B349</f>
         <v>1.2E-2</v>
       </c>
@@ -8457,7 +8461,7 @@
       <c r="F298" s="80"/>
       <c r="G298" s="36"/>
       <c r="H298" s="32"/>
-      <c r="I298" s="134">
+      <c r="I298" s="131">
         <f>'Template Format ANALISIS I'!B350</f>
         <v>0.18</v>
       </c>
@@ -8486,7 +8490,7 @@
       <c r="F299" s="80"/>
       <c r="G299" s="36"/>
       <c r="H299" s="32"/>
-      <c r="I299" s="134">
+      <c r="I299" s="131">
         <f>'Template Format ANALISIS I'!B351</f>
         <v>1.7999999999999999E-2</v>
       </c>
@@ -8515,7 +8519,7 @@
       <c r="F300" s="80"/>
       <c r="G300" s="36"/>
       <c r="H300" s="32"/>
-      <c r="I300" s="134">
+      <c r="I300" s="131">
         <f>'Template Format ANALISIS I'!B352</f>
         <v>1.05</v>
       </c>
@@ -8544,7 +8548,7 @@
       <c r="F301" s="80"/>
       <c r="G301" s="36"/>
       <c r="H301" s="32"/>
-      <c r="I301" s="134">
+      <c r="I301" s="131">
         <f>'Template Format ANALISIS I'!B353</f>
         <v>0.01</v>
       </c>
@@ -8573,7 +8577,7 @@
       <c r="F302" s="80"/>
       <c r="G302" s="36"/>
       <c r="H302" s="32"/>
-      <c r="I302" s="134"/>
+      <c r="I302" s="131"/>
       <c r="J302" s="80"/>
       <c r="K302" s="80" t="str">
         <f>'Template Format ANALISIS I'!D354</f>
@@ -8793,14 +8797,14 @@
       <c r="E314" s="11">
         <v>423</v>
       </c>
-      <c r="F314" s="114">
+      <c r="F314" s="111">
         <v>148753</v>
       </c>
       <c r="G314" s="36">
         <f>F314*E314</f>
         <v>62922519</v>
       </c>
-      <c r="I314" s="125">
+      <c r="I314" s="122">
         <v>5</v>
       </c>
       <c r="J314" s="13" t="s">
@@ -8809,7 +8813,7 @@
       <c r="K314" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L314" s="124">
+      <c r="L314" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -9599,7 +9603,7 @@
       <c r="E349" s="11">
         <v>23.687999999999999</v>
       </c>
-      <c r="F349" s="114">
+      <c r="F349" s="111">
         <f>'Template Format ANALISIS I'!F366 - 55368</f>
         <v>249057</v>
       </c>
@@ -9803,14 +9807,14 @@
       <c r="E359" s="11">
         <v>4</v>
       </c>
-      <c r="F359" s="114">
+      <c r="F359" s="111">
         <v>14000000</v>
       </c>
       <c r="G359" s="36">
         <f>F359*E359</f>
         <v>56000000</v>
       </c>
-      <c r="I359" s="116">
+      <c r="I359" s="113">
         <v>0.5</v>
       </c>
       <c r="J359" s="42" t="s">
@@ -9819,7 +9823,7 @@
       <c r="K359" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="L359" s="114">
+      <c r="L359" s="111">
         <v>110000</v>
       </c>
       <c r="M359" s="44"/>
@@ -10578,7 +10582,7 @@
       <c r="E394" s="57">
         <v>2</v>
       </c>
-      <c r="F394" s="135">
+      <c r="F394" s="132">
         <f>'Template Format ANALISIS I'!F376 - 132266</f>
         <v>40535.200000000012</v>
       </c>
@@ -10587,7 +10591,7 @@
         <v>81070.400000000023</v>
       </c>
       <c r="H394" s="59"/>
-      <c r="I394" s="138">
+      <c r="I394" s="135">
         <f>'Template Format ANALISIS I'!B369</f>
         <v>8.1000000000000003E-2</v>
       </c>
@@ -10614,7 +10618,7 @@
       <c r="F395" s="76"/>
       <c r="G395" s="51"/>
       <c r="H395" s="59"/>
-      <c r="I395" s="138">
+      <c r="I395" s="135">
         <f>'Template Format ANALISIS I'!B370</f>
         <v>4.1000000000000003E-3</v>
       </c>
@@ -10641,7 +10645,7 @@
       <c r="F396" s="76"/>
       <c r="G396" s="51"/>
       <c r="H396" s="59"/>
-      <c r="I396" s="138">
+      <c r="I396" s="135">
         <f>'Template Format ANALISIS I'!B371</f>
         <v>0.13500000000000001</v>
       </c>
@@ -10668,7 +10672,7 @@
       <c r="F397" s="76"/>
       <c r="G397" s="51"/>
       <c r="H397" s="59"/>
-      <c r="I397" s="138">
+      <c r="I397" s="135">
         <f>'Template Format ANALISIS I'!B372</f>
         <v>1.35E-2</v>
       </c>
@@ -10695,7 +10699,7 @@
       <c r="F398" s="76"/>
       <c r="G398" s="51"/>
       <c r="H398" s="59"/>
-      <c r="I398" s="138">
+      <c r="I398" s="135">
         <f>'Template Format ANALISIS I'!B373</f>
         <v>1</v>
       </c>
@@ -10722,7 +10726,7 @@
       <c r="F399" s="76"/>
       <c r="G399" s="51"/>
       <c r="H399" s="59"/>
-      <c r="I399" s="138">
+      <c r="I399" s="135">
         <f>'Template Format ANALISIS I'!B374</f>
         <v>1</v>
       </c>
@@ -10749,7 +10753,7 @@
       <c r="F400" s="76"/>
       <c r="G400" s="51"/>
       <c r="H400" s="59"/>
-      <c r="I400" s="138"/>
+      <c r="I400" s="135"/>
       <c r="J400" s="76"/>
       <c r="K400" s="76" t="str">
         <f>'Template Format ANALISIS I'!D375</f>
@@ -11244,7 +11248,7 @@
       <c r="E420" s="53">
         <v>1</v>
       </c>
-      <c r="F420" s="136">
+      <c r="F420" s="133">
         <v>35000000</v>
       </c>
       <c r="G420" s="51">
@@ -11252,7 +11256,7 @@
         <v>35000000</v>
       </c>
       <c r="H420" s="54"/>
-      <c r="I420" s="137">
+      <c r="I420" s="134">
         <v>0.5</v>
       </c>
       <c r="J420" s="38" t="s">
@@ -11261,7 +11265,7 @@
       <c r="K420" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="L420" s="141">
+      <c r="L420" s="138">
         <v>110000</v>
       </c>
       <c r="M420" s="51"/>
@@ -11288,10 +11292,10 @@
       </c>
     </row>
     <row r="423" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B423" s="139" t="s">
+      <c r="B423" s="136" t="s">
         <v>225</v>
       </c>
-      <c r="C423" s="140" t="s">
+      <c r="C423" s="137" t="s">
         <v>226</v>
       </c>
     </row>
@@ -11316,7 +11320,7 @@
       <c r="E425" s="11">
         <v>13.32</v>
       </c>
-      <c r="F425" s="115">
+      <c r="F425" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -11445,7 +11449,7 @@
       <c r="E431" s="11">
         <v>3328.51</v>
       </c>
-      <c r="F431" s="115">
+      <c r="F431" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -11598,8 +11602,8 @@
       <c r="B437" s="71"/>
       <c r="C437" s="10"/>
       <c r="I437" s="26"/>
-      <c r="J437" s="118"/>
-      <c r="K437" s="118"/>
+      <c r="J437" s="115"/>
+      <c r="K437" s="115"/>
       <c r="L437" s="74"/>
       <c r="M437" s="44"/>
     </row>
@@ -11616,7 +11620,7 @@
       <c r="E438" s="11">
         <v>122.1</v>
       </c>
-      <c r="F438" s="115">
+      <c r="F438" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -11824,7 +11828,7 @@
       <c r="E448" s="11">
         <v>6.03</v>
       </c>
-      <c r="F448" s="115">
+      <c r="F448" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -11953,7 +11957,7 @@
       <c r="E454" s="11">
         <v>1207.5999999999999</v>
       </c>
-      <c r="F454" s="115">
+      <c r="F454" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -12106,8 +12110,8 @@
       <c r="B460" s="71"/>
       <c r="C460" s="10"/>
       <c r="I460" s="26"/>
-      <c r="J460" s="118"/>
-      <c r="K460" s="118"/>
+      <c r="J460" s="115"/>
+      <c r="K460" s="115"/>
       <c r="L460" s="74"/>
       <c r="M460" s="44"/>
     </row>
@@ -12124,7 +12128,7 @@
       <c r="E461" s="11">
         <v>60.26</v>
       </c>
-      <c r="F461" s="115">
+      <c r="F461" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -12332,7 +12336,7 @@
       <c r="E471" s="11">
         <v>2.67</v>
       </c>
-      <c r="F471" s="115">
+      <c r="F471" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -12461,7 +12465,7 @@
       <c r="E477" s="11">
         <v>908.72</v>
       </c>
-      <c r="F477" s="115">
+      <c r="F477" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -12614,8 +12618,8 @@
       <c r="B483" s="71"/>
       <c r="C483" s="10"/>
       <c r="I483" s="26"/>
-      <c r="J483" s="118"/>
-      <c r="K483" s="118"/>
+      <c r="J483" s="115"/>
+      <c r="K483" s="115"/>
       <c r="L483" s="74"/>
       <c r="M483" s="44"/>
     </row>
@@ -12632,7 +12636,7 @@
       <c r="E484" s="11">
         <v>47.47</v>
       </c>
-      <c r="F484" s="115">
+      <c r="F484" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -12840,7 +12844,7 @@
       <c r="E494" s="11">
         <v>9.6</v>
       </c>
-      <c r="F494" s="115">
+      <c r="F494" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -12969,7 +12973,7 @@
       <c r="E500" s="11">
         <v>3762.33</v>
       </c>
-      <c r="F500" s="115">
+      <c r="F500" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -13122,8 +13126,8 @@
       <c r="B506" s="71"/>
       <c r="C506" s="10"/>
       <c r="I506" s="26"/>
-      <c r="J506" s="118"/>
-      <c r="K506" s="118"/>
+      <c r="J506" s="115"/>
+      <c r="K506" s="115"/>
       <c r="L506" s="74"/>
       <c r="M506" s="44"/>
     </row>
@@ -13140,7 +13144,7 @@
       <c r="E507" s="11">
         <v>108.8</v>
       </c>
-      <c r="F507" s="115">
+      <c r="F507" s="112">
         <f>'Template Format ANALISIS I'!F289 + 179612</f>
         <v>481547</v>
       </c>
@@ -13348,7 +13352,7 @@
       <c r="E517" s="11">
         <v>22.96</v>
       </c>
-      <c r="F517" s="115">
+      <c r="F517" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -13482,14 +13486,14 @@
       <c r="E523" s="11">
         <v>191.34</v>
       </c>
-      <c r="F523" s="114">
+      <c r="F523" s="111">
         <v>220000</v>
       </c>
       <c r="G523" s="12">
         <f>F523*E523</f>
         <v>42094800</v>
       </c>
-      <c r="I523" s="116">
+      <c r="I523" s="113">
         <v>0.5</v>
       </c>
       <c r="J523" s="13" t="s">
@@ -13498,7 +13502,7 @@
       <c r="K523" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L523" s="124">
+      <c r="L523" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -13519,14 +13523,14 @@
       <c r="E525" s="11">
         <v>191.34</v>
       </c>
-      <c r="F525" s="114">
+      <c r="F525" s="111">
         <v>240000</v>
       </c>
       <c r="G525" s="12">
         <f>F525*E525</f>
         <v>45921600</v>
       </c>
-      <c r="I525" s="116">
+      <c r="I525" s="113">
         <v>0.5</v>
       </c>
       <c r="J525" s="13" t="s">
@@ -13535,7 +13539,7 @@
       <c r="K525" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L525" s="124">
+      <c r="L525" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -13558,7 +13562,7 @@
       <c r="E527" s="11">
         <v>191.34</v>
       </c>
-      <c r="F527" s="115">
+      <c r="F527" s="112">
         <f>'Template Format ANALISIS I'!F289 + 132312</f>
         <v>434247</v>
       </c>
@@ -13758,7 +13762,7 @@
       <c r="E536" s="11">
         <v>74.8</v>
       </c>
-      <c r="F536" s="114">
+      <c r="F536" s="111">
         <f>'Template Format ANALISIS I'!F306 - 29795.75</f>
         <v>119818</v>
       </c>
@@ -14082,7 +14086,7 @@
       <c r="E551" s="11">
         <v>93.78</v>
       </c>
-      <c r="F551" s="114">
+      <c r="F551" s="111">
         <f>'Template Format ANALISIS I'!F323 - 642.5</f>
         <v>149084</v>
       </c>
@@ -14388,8 +14392,8 @@
       </c>
     </row>
     <row r="565" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B565" s="139"/>
-      <c r="C565" s="140"/>
+      <c r="B565" s="136"/>
+      <c r="C565" s="137"/>
     </row>
     <row r="566" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B566" s="71" t="s">
@@ -14412,14 +14416,14 @@
       <c r="E567" s="11">
         <v>377.71</v>
       </c>
-      <c r="F567" s="114">
+      <c r="F567" s="111">
         <v>148753</v>
       </c>
       <c r="G567" s="36">
         <f>F567*E567</f>
         <v>56185495.629999995</v>
       </c>
-      <c r="I567" s="125">
+      <c r="I567" s="122">
         <v>5</v>
       </c>
       <c r="J567" s="13" t="s">
@@ -14428,7 +14432,7 @@
       <c r="K567" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L567" s="124">
+      <c r="L567" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -15122,7 +15126,7 @@
       <c r="E602" s="11">
         <v>23.687999999999999</v>
       </c>
-      <c r="F602" s="114">
+      <c r="F602" s="111">
         <f>'Template Format ANALISIS I'!F366 - 55368</f>
         <v>249057</v>
       </c>
@@ -15326,7 +15330,7 @@
       <c r="E612" s="35">
         <v>220.78</v>
       </c>
-      <c r="F612" s="113">
+      <c r="F612" s="110">
         <f>'Template Format ANALISIS I'!F334 - 291381</f>
         <v>293104</v>
       </c>
@@ -15355,7 +15359,7 @@
         <f>'Template Format ANALISIS I'!F326</f>
         <v>110000</v>
       </c>
-      <c r="V612" s="140"/>
+      <c r="V612" s="137"/>
       <c r="W612" s="6"/>
       <c r="X612" s="7"/>
     </row>
@@ -15387,8 +15391,8 @@
         <f>'Template Format ANALISIS I'!F327</f>
         <v>5400</v>
       </c>
-      <c r="V613" s="117"/>
-      <c r="W613" s="118"/>
+      <c r="V613" s="114"/>
+      <c r="W613" s="115"/>
       <c r="X613" s="7"/>
     </row>
     <row r="614" spans="2:24" x14ac:dyDescent="0.3">
@@ -15419,8 +15423,8 @@
         <f>'Template Format ANALISIS I'!F328</f>
         <v>58500</v>
       </c>
-      <c r="V614" s="140"/>
-      <c r="W614" s="144"/>
+      <c r="V614" s="137"/>
+      <c r="W614" s="141"/>
       <c r="X614" s="7"/>
     </row>
     <row r="615" spans="2:24" x14ac:dyDescent="0.3">
@@ -15586,7 +15590,7 @@
       <c r="E621" s="35">
         <v>9.68</v>
       </c>
-      <c r="F621" s="113">
+      <c r="F621" s="110">
         <f>'Template Format ANALISIS I'!F345 - 66973</f>
         <v>249057</v>
       </c>
@@ -15829,10 +15833,10 @@
       <c r="E630" s="11">
         <v>15.6</v>
       </c>
-      <c r="F630" s="114">
+      <c r="F630" s="111">
         <v>120000</v>
       </c>
-      <c r="I630" s="125">
+      <c r="I630" s="122">
         <v>5</v>
       </c>
       <c r="J630" s="13" t="s">
@@ -15841,7 +15845,7 @@
       <c r="K630" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L630" s="124">
+      <c r="L630" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -16084,7 +16088,7 @@
       <c r="E641" s="35">
         <v>14</v>
       </c>
-      <c r="F641" s="113">
+      <c r="F641" s="110">
         <f>'Template Format ANALISIS I'!F355 - 26939</f>
         <v>43857</v>
       </c>
@@ -16093,15 +16097,15 @@
         <v>613998</v>
       </c>
       <c r="H641" s="32"/>
-      <c r="I641" s="134">
+      <c r="I641" s="131">
         <f>'Template Format ANALISIS I'!B348</f>
         <v>0.12</v>
       </c>
-      <c r="J641" s="134" t="str">
+      <c r="J641" s="131" t="str">
         <f>'Template Format ANALISIS I'!C348</f>
         <v>OH</v>
       </c>
-      <c r="K641" s="134" t="str">
+      <c r="K641" s="131" t="str">
         <f>'Template Format ANALISIS I'!D348</f>
         <v xml:space="preserve">Pekerja </v>
       </c>
@@ -16122,15 +16126,15 @@
       <c r="F642" s="80"/>
       <c r="G642" s="36"/>
       <c r="H642" s="32"/>
-      <c r="I642" s="134">
+      <c r="I642" s="131">
         <f>'Template Format ANALISIS I'!B349</f>
         <v>1.2E-2</v>
       </c>
-      <c r="J642" s="134" t="str">
+      <c r="J642" s="131" t="str">
         <f>'Template Format ANALISIS I'!C349</f>
         <v>OH</v>
       </c>
-      <c r="K642" s="134" t="str">
+      <c r="K642" s="131" t="str">
         <f>'Template Format ANALISIS I'!D349</f>
         <v>Mandor</v>
       </c>
@@ -16151,15 +16155,15 @@
       <c r="F643" s="80"/>
       <c r="G643" s="36"/>
       <c r="H643" s="32"/>
-      <c r="I643" s="134">
+      <c r="I643" s="131">
         <f>'Template Format ANALISIS I'!B350</f>
         <v>0.18</v>
       </c>
-      <c r="J643" s="134" t="str">
+      <c r="J643" s="131" t="str">
         <f>'Template Format ANALISIS I'!C350</f>
         <v>OH</v>
       </c>
-      <c r="K643" s="134" t="str">
+      <c r="K643" s="131" t="str">
         <f>'Template Format ANALISIS I'!D350</f>
         <v>Tukang</v>
       </c>
@@ -16180,15 +16184,15 @@
       <c r="F644" s="80"/>
       <c r="G644" s="36"/>
       <c r="H644" s="32"/>
-      <c r="I644" s="134">
+      <c r="I644" s="131">
         <f>'Template Format ANALISIS I'!B351</f>
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J644" s="134" t="str">
+      <c r="J644" s="131" t="str">
         <f>'Template Format ANALISIS I'!C351</f>
         <v>OH</v>
       </c>
-      <c r="K644" s="134" t="str">
+      <c r="K644" s="131" t="str">
         <f>'Template Format ANALISIS I'!D351</f>
         <v>Kepala Tukang</v>
       </c>
@@ -16209,15 +16213,15 @@
       <c r="F645" s="80"/>
       <c r="G645" s="36"/>
       <c r="H645" s="32"/>
-      <c r="I645" s="134">
+      <c r="I645" s="131">
         <f>'Template Format ANALISIS I'!B352</f>
         <v>1.05</v>
       </c>
-      <c r="J645" s="134" t="str">
+      <c r="J645" s="131" t="str">
         <f>'Template Format ANALISIS I'!C352</f>
         <v>M1</v>
       </c>
-      <c r="K645" s="134" t="str">
+      <c r="K645" s="131" t="str">
         <f>'Template Format ANALISIS I'!D352</f>
         <v>Gypsum Profil</v>
       </c>
@@ -16238,15 +16242,15 @@
       <c r="F646" s="80"/>
       <c r="G646" s="36"/>
       <c r="H646" s="32"/>
-      <c r="I646" s="134">
+      <c r="I646" s="131">
         <f>'Template Format ANALISIS I'!B353</f>
         <v>0.01</v>
       </c>
-      <c r="J646" s="134" t="str">
+      <c r="J646" s="131" t="str">
         <f>'Template Format ANALISIS I'!C353</f>
         <v xml:space="preserve">Doz </v>
       </c>
-      <c r="K646" s="134" t="str">
+      <c r="K646" s="131" t="str">
         <f>'Template Format ANALISIS I'!D353</f>
         <v>Paku/sekrup</v>
       </c>
@@ -16267,9 +16271,9 @@
       <c r="F647" s="80"/>
       <c r="G647" s="36"/>
       <c r="H647" s="32"/>
-      <c r="I647" s="134"/>
-      <c r="J647" s="134"/>
-      <c r="K647" s="134" t="str">
+      <c r="I647" s="131"/>
+      <c r="J647" s="131"/>
+      <c r="K647" s="131" t="str">
         <f>'Template Format ANALISIS I'!D354</f>
         <v>B.U &amp; Kentungan (10%)</v>
       </c>
@@ -17220,7 +17224,7 @@
       <c r="E691" s="57">
         <v>2</v>
       </c>
-      <c r="F691" s="135">
+      <c r="F691" s="132">
         <f>'Template Format ANALISIS I'!F376 - 132266</f>
         <v>40535.200000000012</v>
       </c>
@@ -17229,15 +17233,15 @@
         <v>81070.400000000023</v>
       </c>
       <c r="H691" s="59"/>
-      <c r="I691" s="138">
+      <c r="I691" s="135">
         <f>'Template Format ANALISIS I'!B369</f>
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="J691" s="138" t="str">
+      <c r="J691" s="135" t="str">
         <f>'Template Format ANALISIS I'!C369</f>
         <v>OH</v>
       </c>
-      <c r="K691" s="138" t="str">
+      <c r="K691" s="135" t="str">
         <f>'Template Format ANALISIS I'!D369</f>
         <v xml:space="preserve">Pekerja </v>
       </c>
@@ -17256,15 +17260,15 @@
       <c r="F692" s="76"/>
       <c r="G692" s="51"/>
       <c r="H692" s="59"/>
-      <c r="I692" s="138">
+      <c r="I692" s="135">
         <f>'Template Format ANALISIS I'!B370</f>
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="J692" s="138" t="str">
+      <c r="J692" s="135" t="str">
         <f>'Template Format ANALISIS I'!C370</f>
         <v>OH</v>
       </c>
-      <c r="K692" s="138" t="str">
+      <c r="K692" s="135" t="str">
         <f>'Template Format ANALISIS I'!D370</f>
         <v>Mandor</v>
       </c>
@@ -17283,15 +17287,15 @@
       <c r="F693" s="76"/>
       <c r="G693" s="51"/>
       <c r="H693" s="59"/>
-      <c r="I693" s="138">
+      <c r="I693" s="135">
         <f>'Template Format ANALISIS I'!B371</f>
         <v>0.13500000000000001</v>
       </c>
-      <c r="J693" s="138" t="str">
+      <c r="J693" s="135" t="str">
         <f>'Template Format ANALISIS I'!C371</f>
         <v>OH</v>
       </c>
-      <c r="K693" s="138" t="str">
+      <c r="K693" s="135" t="str">
         <f>'Template Format ANALISIS I'!D371</f>
         <v xml:space="preserve">Tukang </v>
       </c>
@@ -17310,15 +17314,15 @@
       <c r="F694" s="76"/>
       <c r="G694" s="51"/>
       <c r="H694" s="59"/>
-      <c r="I694" s="138">
+      <c r="I694" s="135">
         <f>'Template Format ANALISIS I'!B372</f>
         <v>1.35E-2</v>
       </c>
-      <c r="J694" s="138" t="str">
+      <c r="J694" s="135" t="str">
         <f>'Template Format ANALISIS I'!C372</f>
         <v>OH</v>
       </c>
-      <c r="K694" s="138" t="str">
+      <c r="K694" s="135" t="str">
         <f>'Template Format ANALISIS I'!D372</f>
         <v>Kepala Tukang</v>
       </c>
@@ -17337,15 +17341,15 @@
       <c r="F695" s="76"/>
       <c r="G695" s="51"/>
       <c r="H695" s="59"/>
-      <c r="I695" s="138">
+      <c r="I695" s="135">
         <f>'Template Format ANALISIS I'!B373</f>
         <v>1</v>
       </c>
-      <c r="J695" s="138" t="str">
+      <c r="J695" s="135" t="str">
         <f>'Template Format ANALISIS I'!C373</f>
         <v>Bh</v>
       </c>
-      <c r="K695" s="138" t="str">
+      <c r="K695" s="135" t="str">
         <f>'Template Format ANALISIS I'!D373</f>
         <v>Floordrain Besi</v>
       </c>
@@ -17364,12 +17368,12 @@
       <c r="F696" s="76"/>
       <c r="G696" s="51"/>
       <c r="H696" s="59"/>
-      <c r="I696" s="138">
+      <c r="I696" s="135">
         <f>'Template Format ANALISIS I'!B374</f>
         <v>1</v>
       </c>
-      <c r="J696" s="138"/>
-      <c r="K696" s="138" t="str">
+      <c r="J696" s="135"/>
+      <c r="K696" s="135" t="str">
         <f>'Template Format ANALISIS I'!D374</f>
         <v>Perlengkapan</v>
       </c>
@@ -17388,9 +17392,9 @@
       <c r="F697" s="76"/>
       <c r="G697" s="51"/>
       <c r="H697" s="59"/>
-      <c r="I697" s="138"/>
-      <c r="J697" s="138"/>
-      <c r="K697" s="138" t="str">
+      <c r="I697" s="135"/>
+      <c r="J697" s="135"/>
+      <c r="K697" s="135" t="str">
         <f>'Template Format ANALISIS I'!D375</f>
         <v>B.U &amp; Kentungan (10%)</v>
       </c>
@@ -17422,10 +17426,10 @@
       </c>
     </row>
     <row r="700" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B700" s="139" t="s">
+      <c r="B700" s="136" t="s">
         <v>237</v>
       </c>
-      <c r="C700" s="140" t="s">
+      <c r="C700" s="137" t="s">
         <v>226</v>
       </c>
     </row>
@@ -17450,7 +17454,7 @@
       <c r="E702" s="11">
         <v>13.32</v>
       </c>
-      <c r="F702" s="115">
+      <c r="F702" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -17579,7 +17583,7 @@
       <c r="E708" s="11">
         <v>3328.51</v>
       </c>
-      <c r="F708" s="115">
+      <c r="F708" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -17732,8 +17736,8 @@
       <c r="B714" s="71"/>
       <c r="C714" s="10"/>
       <c r="I714" s="26"/>
-      <c r="J714" s="118"/>
-      <c r="K714" s="118"/>
+      <c r="J714" s="115"/>
+      <c r="K714" s="115"/>
       <c r="L714" s="74"/>
       <c r="M714" s="44"/>
     </row>
@@ -17750,7 +17754,7 @@
       <c r="E715" s="11">
         <v>122.1</v>
       </c>
-      <c r="F715" s="115">
+      <c r="F715" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -17958,7 +17962,7 @@
       <c r="E725" s="11">
         <v>6.03</v>
       </c>
-      <c r="F725" s="115">
+      <c r="F725" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -18089,7 +18093,7 @@
       <c r="E731" s="11">
         <v>1207.5999999999999</v>
       </c>
-      <c r="F731" s="115">
+      <c r="F731" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -18248,8 +18252,8 @@
       <c r="B737" s="71"/>
       <c r="C737" s="10"/>
       <c r="I737" s="26"/>
-      <c r="J737" s="118"/>
-      <c r="K737" s="118"/>
+      <c r="J737" s="115"/>
+      <c r="K737" s="115"/>
       <c r="L737" s="74"/>
       <c r="M737" s="44"/>
       <c r="N737" s="1"/>
@@ -18267,7 +18271,7 @@
       <c r="E738" s="11">
         <v>60.26</v>
       </c>
-      <c r="F738" s="115">
+      <c r="F738" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -18483,7 +18487,7 @@
       <c r="E748" s="11">
         <v>2.67</v>
       </c>
-      <c r="F748" s="115">
+      <c r="F748" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -18617,7 +18621,7 @@
       <c r="E754" s="11">
         <v>768.2</v>
       </c>
-      <c r="F754" s="115">
+      <c r="F754" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -18776,8 +18780,8 @@
       <c r="B760" s="71"/>
       <c r="C760" s="10"/>
       <c r="I760" s="26"/>
-      <c r="J760" s="118"/>
-      <c r="K760" s="118"/>
+      <c r="J760" s="115"/>
+      <c r="K760" s="115"/>
       <c r="L760" s="74"/>
       <c r="M760" s="44"/>
     </row>
@@ -18794,7 +18798,7 @@
       <c r="E761" s="11">
         <v>40.119999999999997</v>
       </c>
-      <c r="F761" s="115">
+      <c r="F761" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -19003,7 +19007,7 @@
       <c r="E771" s="11">
         <v>9.6</v>
       </c>
-      <c r="F771" s="115">
+      <c r="F771" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -19132,7 +19136,7 @@
       <c r="E777" s="11">
         <v>3762.33</v>
       </c>
-      <c r="F777" s="115">
+      <c r="F777" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -19285,8 +19289,8 @@
       <c r="B783" s="71"/>
       <c r="C783" s="10"/>
       <c r="I783" s="26"/>
-      <c r="J783" s="118"/>
-      <c r="K783" s="118"/>
+      <c r="J783" s="115"/>
+      <c r="K783" s="115"/>
       <c r="L783" s="74"/>
       <c r="M783" s="44"/>
     </row>
@@ -19303,7 +19307,7 @@
       <c r="E784" s="11">
         <v>108.8</v>
       </c>
-      <c r="F784" s="115">
+      <c r="F784" s="112">
         <f>'Template Format ANALISIS I'!F289 + 179612</f>
         <v>481547</v>
       </c>
@@ -19511,7 +19515,7 @@
       <c r="E794" s="11">
         <v>22.96</v>
       </c>
-      <c r="F794" s="115">
+      <c r="F794" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -19645,14 +19649,14 @@
       <c r="E800" s="11">
         <v>191.34</v>
       </c>
-      <c r="F800" s="114">
+      <c r="F800" s="111">
         <v>220000</v>
       </c>
       <c r="G800" s="12">
         <f>F800*E800</f>
         <v>42094800</v>
       </c>
-      <c r="I800" s="116">
+      <c r="I800" s="113">
         <v>0.5</v>
       </c>
       <c r="J800" s="13" t="s">
@@ -19661,7 +19665,7 @@
       <c r="K800" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L800" s="124">
+      <c r="L800" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -19682,14 +19686,14 @@
       <c r="E802" s="11">
         <v>191.34</v>
       </c>
-      <c r="F802" s="114">
+      <c r="F802" s="111">
         <v>240000</v>
       </c>
       <c r="G802" s="12">
         <f>F802*E802</f>
         <v>45921600</v>
       </c>
-      <c r="I802" s="116">
+      <c r="I802" s="113">
         <v>0.5</v>
       </c>
       <c r="J802" s="13" t="s">
@@ -19698,7 +19702,7 @@
       <c r="K802" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L802" s="124">
+      <c r="L802" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -19721,7 +19725,7 @@
       <c r="E804" s="11">
         <v>191.34</v>
       </c>
-      <c r="F804" s="115">
+      <c r="F804" s="112">
         <f>'Template Format ANALISIS I'!F289 + 132312</f>
         <v>434247</v>
       </c>
@@ -19921,7 +19925,7 @@
       <c r="E813" s="11">
         <v>74.8</v>
       </c>
-      <c r="F813" s="114">
+      <c r="F813" s="111">
         <f>'Template Format ANALISIS I'!F306 - 29795.75</f>
         <v>119818</v>
       </c>
@@ -20245,7 +20249,7 @@
       <c r="E828" s="11">
         <v>93.78</v>
       </c>
-      <c r="F828" s="114">
+      <c r="F828" s="111">
         <f>'Template Format ANALISIS I'!F323 - 642.5</f>
         <v>149084</v>
       </c>
@@ -20551,8 +20555,8 @@
       </c>
     </row>
     <row r="842" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B842" s="139"/>
-      <c r="C842" s="140"/>
+      <c r="B842" s="136"/>
+      <c r="C842" s="137"/>
     </row>
     <row r="843" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B843" s="72" t="s">
@@ -20575,14 +20579,14 @@
       <c r="E844" s="11">
         <v>342.57</v>
       </c>
-      <c r="F844" s="114">
+      <c r="F844" s="111">
         <v>148753</v>
       </c>
       <c r="G844" s="36">
         <f>F844*E844</f>
         <v>50958315.210000001</v>
       </c>
-      <c r="I844" s="125">
+      <c r="I844" s="122">
         <v>5</v>
       </c>
       <c r="J844" s="13" t="s">
@@ -20591,7 +20595,7 @@
       <c r="K844" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L844" s="124">
+      <c r="L844" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -21305,7 +21309,7 @@
       <c r="E879" s="11">
         <v>23.687999999999999</v>
       </c>
-      <c r="F879" s="114">
+      <c r="F879" s="111">
         <f>'Template Format ANALISIS I'!F366 - 55368</f>
         <v>249057</v>
       </c>
@@ -21509,7 +21513,7 @@
       <c r="E889" s="35">
         <v>220.78</v>
       </c>
-      <c r="F889" s="113">
+      <c r="F889" s="110">
         <f>'Template Format ANALISIS I'!F334 - 291381</f>
         <v>293104</v>
       </c>
@@ -21760,7 +21764,7 @@
       <c r="E898" s="35">
         <v>9.68</v>
       </c>
-      <c r="F898" s="113">
+      <c r="F898" s="110">
         <f>'Template Format ANALISIS I'!F345 - 66973</f>
         <v>249057</v>
       </c>
@@ -22000,14 +22004,14 @@
       <c r="E907" s="11">
         <v>15.6</v>
       </c>
-      <c r="F907" s="114">
+      <c r="F907" s="111">
         <v>120000</v>
       </c>
       <c r="G907" s="36">
         <f>F907*E907</f>
         <v>1872000</v>
       </c>
-      <c r="I907" s="125">
+      <c r="I907" s="122">
         <v>5</v>
       </c>
       <c r="J907" s="13" t="s">
@@ -22016,7 +22020,7 @@
       <c r="K907" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L907" s="124">
+      <c r="L907" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -22256,7 +22260,7 @@
       <c r="E918" s="35">
         <v>14</v>
       </c>
-      <c r="F918" s="113">
+      <c r="F918" s="110">
         <f>'Template Format ANALISIS I'!F355 - 26939</f>
         <v>43857</v>
       </c>
@@ -22265,15 +22269,15 @@
         <v>613998</v>
       </c>
       <c r="H918" s="32"/>
-      <c r="I918" s="134">
+      <c r="I918" s="131">
         <f>'Template Format ANALISIS I'!B348</f>
         <v>0.12</v>
       </c>
-      <c r="J918" s="134" t="str">
+      <c r="J918" s="131" t="str">
         <f>'Template Format ANALISIS I'!C348</f>
         <v>OH</v>
       </c>
-      <c r="K918" s="134" t="str">
+      <c r="K918" s="131" t="str">
         <f>'Template Format ANALISIS I'!D348</f>
         <v xml:space="preserve">Pekerja </v>
       </c>
@@ -22294,15 +22298,15 @@
       <c r="F919" s="80"/>
       <c r="G919" s="36"/>
       <c r="H919" s="32"/>
-      <c r="I919" s="134">
+      <c r="I919" s="131">
         <f>'Template Format ANALISIS I'!B349</f>
         <v>1.2E-2</v>
       </c>
-      <c r="J919" s="134" t="str">
+      <c r="J919" s="131" t="str">
         <f>'Template Format ANALISIS I'!C349</f>
         <v>OH</v>
       </c>
-      <c r="K919" s="134" t="str">
+      <c r="K919" s="131" t="str">
         <f>'Template Format ANALISIS I'!D349</f>
         <v>Mandor</v>
       </c>
@@ -22323,15 +22327,15 @@
       <c r="F920" s="80"/>
       <c r="G920" s="36"/>
       <c r="H920" s="32"/>
-      <c r="I920" s="134">
+      <c r="I920" s="131">
         <f>'Template Format ANALISIS I'!B350</f>
         <v>0.18</v>
       </c>
-      <c r="J920" s="134" t="str">
+      <c r="J920" s="131" t="str">
         <f>'Template Format ANALISIS I'!C350</f>
         <v>OH</v>
       </c>
-      <c r="K920" s="134" t="str">
+      <c r="K920" s="131" t="str">
         <f>'Template Format ANALISIS I'!D350</f>
         <v>Tukang</v>
       </c>
@@ -22352,15 +22356,15 @@
       <c r="F921" s="80"/>
       <c r="G921" s="36"/>
       <c r="H921" s="32"/>
-      <c r="I921" s="134">
+      <c r="I921" s="131">
         <f>'Template Format ANALISIS I'!B351</f>
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J921" s="134" t="str">
+      <c r="J921" s="131" t="str">
         <f>'Template Format ANALISIS I'!C351</f>
         <v>OH</v>
       </c>
-      <c r="K921" s="134" t="str">
+      <c r="K921" s="131" t="str">
         <f>'Template Format ANALISIS I'!D351</f>
         <v>Kepala Tukang</v>
       </c>
@@ -22381,15 +22385,15 @@
       <c r="F922" s="80"/>
       <c r="G922" s="36"/>
       <c r="H922" s="32"/>
-      <c r="I922" s="134">
+      <c r="I922" s="131">
         <f>'Template Format ANALISIS I'!B352</f>
         <v>1.05</v>
       </c>
-      <c r="J922" s="134" t="str">
+      <c r="J922" s="131" t="str">
         <f>'Template Format ANALISIS I'!C352</f>
         <v>M1</v>
       </c>
-      <c r="K922" s="134" t="str">
+      <c r="K922" s="131" t="str">
         <f>'Template Format ANALISIS I'!D352</f>
         <v>Gypsum Profil</v>
       </c>
@@ -22410,15 +22414,15 @@
       <c r="F923" s="80"/>
       <c r="G923" s="36"/>
       <c r="H923" s="32"/>
-      <c r="I923" s="134">
+      <c r="I923" s="131">
         <f>'Template Format ANALISIS I'!B353</f>
         <v>0.01</v>
       </c>
-      <c r="J923" s="134" t="str">
+      <c r="J923" s="131" t="str">
         <f>'Template Format ANALISIS I'!C353</f>
         <v xml:space="preserve">Doz </v>
       </c>
-      <c r="K923" s="134" t="str">
+      <c r="K923" s="131" t="str">
         <f>'Template Format ANALISIS I'!D353</f>
         <v>Paku/sekrup</v>
       </c>
@@ -22439,9 +22443,9 @@
       <c r="F924" s="80"/>
       <c r="G924" s="36"/>
       <c r="H924" s="32"/>
-      <c r="I924" s="134"/>
-      <c r="J924" s="134"/>
-      <c r="K924" s="134" t="str">
+      <c r="I924" s="131"/>
+      <c r="J924" s="131"/>
+      <c r="K924" s="131" t="str">
         <f>'Template Format ANALISIS I'!D354</f>
         <v>B.U &amp; Kentungan (10%)</v>
       </c>
@@ -23362,7 +23366,7 @@
       <c r="E968" s="57">
         <v>2</v>
       </c>
-      <c r="F968" s="135">
+      <c r="F968" s="132">
         <f>'Template Format ANALISIS I'!F376 - 132266</f>
         <v>40535.200000000012</v>
       </c>
@@ -23371,15 +23375,15 @@
         <v>81070.400000000023</v>
       </c>
       <c r="H968" s="59"/>
-      <c r="I968" s="138">
+      <c r="I968" s="135">
         <f>'Template Format ANALISIS I'!B369</f>
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="J968" s="138" t="str">
+      <c r="J968" s="135" t="str">
         <f>'Template Format ANALISIS I'!C369</f>
         <v>OH</v>
       </c>
-      <c r="K968" s="138" t="str">
+      <c r="K968" s="135" t="str">
         <f>'Template Format ANALISIS I'!D369</f>
         <v xml:space="preserve">Pekerja </v>
       </c>
@@ -23398,15 +23402,15 @@
       <c r="F969" s="76"/>
       <c r="G969" s="51"/>
       <c r="H969" s="59"/>
-      <c r="I969" s="138">
+      <c r="I969" s="135">
         <f>'Template Format ANALISIS I'!B370</f>
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="J969" s="138" t="str">
+      <c r="J969" s="135" t="str">
         <f>'Template Format ANALISIS I'!C370</f>
         <v>OH</v>
       </c>
-      <c r="K969" s="138" t="str">
+      <c r="K969" s="135" t="str">
         <f>'Template Format ANALISIS I'!D370</f>
         <v>Mandor</v>
       </c>
@@ -23425,15 +23429,15 @@
       <c r="F970" s="76"/>
       <c r="G970" s="51"/>
       <c r="H970" s="59"/>
-      <c r="I970" s="138">
+      <c r="I970" s="135">
         <f>'Template Format ANALISIS I'!B371</f>
         <v>0.13500000000000001</v>
       </c>
-      <c r="J970" s="138" t="str">
+      <c r="J970" s="135" t="str">
         <f>'Template Format ANALISIS I'!C371</f>
         <v>OH</v>
       </c>
-      <c r="K970" s="138" t="str">
+      <c r="K970" s="135" t="str">
         <f>'Template Format ANALISIS I'!D371</f>
         <v xml:space="preserve">Tukang </v>
       </c>
@@ -23452,15 +23456,15 @@
       <c r="F971" s="76"/>
       <c r="G971" s="51"/>
       <c r="H971" s="59"/>
-      <c r="I971" s="138">
+      <c r="I971" s="135">
         <f>'Template Format ANALISIS I'!B372</f>
         <v>1.35E-2</v>
       </c>
-      <c r="J971" s="138" t="str">
+      <c r="J971" s="135" t="str">
         <f>'Template Format ANALISIS I'!C372</f>
         <v>OH</v>
       </c>
-      <c r="K971" s="138" t="str">
+      <c r="K971" s="135" t="str">
         <f>'Template Format ANALISIS I'!D372</f>
         <v>Kepala Tukang</v>
       </c>
@@ -23479,15 +23483,15 @@
       <c r="F972" s="76"/>
       <c r="G972" s="51"/>
       <c r="H972" s="59"/>
-      <c r="I972" s="138">
+      <c r="I972" s="135">
         <f>'Template Format ANALISIS I'!B373</f>
         <v>1</v>
       </c>
-      <c r="J972" s="138" t="str">
+      <c r="J972" s="135" t="str">
         <f>'Template Format ANALISIS I'!C373</f>
         <v>Bh</v>
       </c>
-      <c r="K972" s="138" t="str">
+      <c r="K972" s="135" t="str">
         <f>'Template Format ANALISIS I'!D373</f>
         <v>Floordrain Besi</v>
       </c>
@@ -23506,12 +23510,12 @@
       <c r="F973" s="76"/>
       <c r="G973" s="51"/>
       <c r="H973" s="59"/>
-      <c r="I973" s="138">
+      <c r="I973" s="135">
         <f>'Template Format ANALISIS I'!B374</f>
         <v>1</v>
       </c>
-      <c r="J973" s="138"/>
-      <c r="K973" s="138" t="str">
+      <c r="J973" s="135"/>
+      <c r="K973" s="135" t="str">
         <f>'Template Format ANALISIS I'!D374</f>
         <v>Perlengkapan</v>
       </c>
@@ -23530,9 +23534,9 @@
       <c r="F974" s="76"/>
       <c r="G974" s="51"/>
       <c r="H974" s="59"/>
-      <c r="I974" s="138"/>
-      <c r="J974" s="138"/>
-      <c r="K974" s="138" t="str">
+      <c r="I974" s="135"/>
+      <c r="J974" s="135"/>
+      <c r="K974" s="135" t="str">
         <f>'Template Format ANALISIS I'!D375</f>
         <v>B.U &amp; Kentungan (10%)</v>
       </c>
@@ -23551,10 +23555,10 @@
       </c>
     </row>
     <row r="977" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B977" s="139" t="s">
+      <c r="B977" s="136" t="s">
         <v>239</v>
       </c>
-      <c r="C977" s="140" t="s">
+      <c r="C977" s="137" t="s">
         <v>226</v>
       </c>
     </row>
@@ -23579,7 +23583,7 @@
       <c r="E979" s="11">
         <v>13.32</v>
       </c>
-      <c r="F979" s="115">
+      <c r="F979" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -23708,7 +23712,7 @@
       <c r="E985" s="11">
         <v>3328.51</v>
       </c>
-      <c r="F985" s="115">
+      <c r="F985" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -23861,8 +23865,8 @@
       <c r="B991" s="71"/>
       <c r="C991" s="10"/>
       <c r="I991" s="26"/>
-      <c r="J991" s="118"/>
-      <c r="K991" s="118"/>
+      <c r="J991" s="115"/>
+      <c r="K991" s="115"/>
       <c r="L991" s="74"/>
       <c r="M991" s="44"/>
     </row>
@@ -23879,7 +23883,7 @@
       <c r="E992" s="11">
         <v>122.1</v>
       </c>
-      <c r="F992" s="115">
+      <c r="F992" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -24087,7 +24091,7 @@
       <c r="E1002" s="11">
         <v>6.03</v>
       </c>
-      <c r="F1002" s="115">
+      <c r="F1002" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -24216,7 +24220,7 @@
       <c r="E1008" s="11">
         <v>1207.5999999999999</v>
       </c>
-      <c r="F1008" s="115">
+      <c r="F1008" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -24369,8 +24373,8 @@
       <c r="B1014" s="71"/>
       <c r="C1014" s="10"/>
       <c r="I1014" s="26"/>
-      <c r="J1014" s="118"/>
-      <c r="K1014" s="118"/>
+      <c r="J1014" s="115"/>
+      <c r="K1014" s="115"/>
       <c r="L1014" s="74"/>
       <c r="M1014" s="44"/>
     </row>
@@ -24387,7 +24391,7 @@
       <c r="E1015" s="11">
         <v>60.26</v>
       </c>
-      <c r="F1015" s="115">
+      <c r="F1015" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -24595,7 +24599,7 @@
       <c r="E1025" s="11">
         <v>2.67</v>
       </c>
-      <c r="F1025" s="115">
+      <c r="F1025" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -24724,7 +24728,7 @@
       <c r="E1031" s="11">
         <v>768.2</v>
       </c>
-      <c r="F1031" s="115">
+      <c r="F1031" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -24877,8 +24881,8 @@
       <c r="B1037" s="71"/>
       <c r="C1037" s="10"/>
       <c r="I1037" s="26"/>
-      <c r="J1037" s="118"/>
-      <c r="K1037" s="118"/>
+      <c r="J1037" s="115"/>
+      <c r="K1037" s="115"/>
       <c r="L1037" s="74"/>
       <c r="M1037" s="44"/>
     </row>
@@ -24895,7 +24899,7 @@
       <c r="E1038" s="11">
         <v>40.119999999999997</v>
       </c>
-      <c r="F1038" s="115">
+      <c r="F1038" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -25103,7 +25107,7 @@
       <c r="E1048" s="11">
         <v>9.6</v>
       </c>
-      <c r="F1048" s="115">
+      <c r="F1048" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -25232,7 +25236,7 @@
       <c r="E1054" s="11">
         <v>3762.33</v>
       </c>
-      <c r="F1054" s="115">
+      <c r="F1054" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -25385,8 +25389,8 @@
       <c r="B1060" s="71"/>
       <c r="C1060" s="10"/>
       <c r="I1060" s="26"/>
-      <c r="J1060" s="118"/>
-      <c r="K1060" s="118"/>
+      <c r="J1060" s="115"/>
+      <c r="K1060" s="115"/>
       <c r="L1060" s="74"/>
       <c r="M1060" s="44"/>
     </row>
@@ -25403,7 +25407,7 @@
       <c r="E1061" s="11">
         <v>108.8</v>
       </c>
-      <c r="F1061" s="115">
+      <c r="F1061" s="112">
         <f>'Template Format ANALISIS I'!F289 + 179612</f>
         <v>481547</v>
       </c>
@@ -25611,7 +25615,7 @@
       <c r="E1071" s="11">
         <v>22.96</v>
       </c>
-      <c r="F1071" s="115">
+      <c r="F1071" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -25745,14 +25749,14 @@
       <c r="E1077" s="11">
         <v>191.34</v>
       </c>
-      <c r="F1077" s="114">
+      <c r="F1077" s="111">
         <v>220000</v>
       </c>
       <c r="G1077" s="12">
         <f>F1077*E1077</f>
         <v>42094800</v>
       </c>
-      <c r="I1077" s="116">
+      <c r="I1077" s="113">
         <v>0.5</v>
       </c>
       <c r="J1077" s="13" t="s">
@@ -25761,7 +25765,7 @@
       <c r="K1077" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1077" s="124">
+      <c r="L1077" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -25782,14 +25786,14 @@
       <c r="E1079" s="11">
         <v>191.34</v>
       </c>
-      <c r="F1079" s="114">
+      <c r="F1079" s="111">
         <v>240000</v>
       </c>
       <c r="G1079" s="12">
         <f>F1079*E1079</f>
         <v>45921600</v>
       </c>
-      <c r="I1079" s="116">
+      <c r="I1079" s="113">
         <v>0.5</v>
       </c>
       <c r="J1079" s="13" t="s">
@@ -25798,7 +25802,7 @@
       <c r="K1079" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1079" s="124">
+      <c r="L1079" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -25821,7 +25825,7 @@
       <c r="E1081" s="11">
         <v>191.34</v>
       </c>
-      <c r="F1081" s="115">
+      <c r="F1081" s="112">
         <f>'Template Format ANALISIS I'!F289 + 132312</f>
         <v>434247</v>
       </c>
@@ -26021,7 +26025,7 @@
       <c r="E1090" s="11">
         <v>74.8</v>
       </c>
-      <c r="F1090" s="114">
+      <c r="F1090" s="111">
         <f>'Template Format ANALISIS I'!F306 - 29795.75</f>
         <v>119818</v>
       </c>
@@ -26345,7 +26349,7 @@
       <c r="E1105" s="11">
         <v>93.78</v>
       </c>
-      <c r="F1105" s="114">
+      <c r="F1105" s="111">
         <f>'Template Format ANALISIS I'!F323 - 642.5</f>
         <v>149084</v>
       </c>
@@ -26672,14 +26676,14 @@
       <c r="E1120" s="11">
         <v>342.57</v>
       </c>
-      <c r="F1120" s="114">
+      <c r="F1120" s="111">
         <v>148753</v>
       </c>
       <c r="G1120" s="36">
         <f>F1120*E1120</f>
         <v>50958315.210000001</v>
       </c>
-      <c r="I1120" s="125">
+      <c r="I1120" s="122">
         <v>5</v>
       </c>
       <c r="J1120" s="13" t="s">
@@ -26688,7 +26692,7 @@
       <c r="K1120" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1120" s="124">
+      <c r="L1120" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -26710,7 +26714,7 @@
       <c r="E1122" s="11">
         <v>685.13460000000009</v>
       </c>
-      <c r="F1122" s="142">
+      <c r="F1122" s="139">
         <f>'Template Format ANALISIS I'!F120</f>
         <v>77396</v>
       </c>
@@ -26889,7 +26893,7 @@
       <c r="E1130" s="11">
         <v>685.13460000000009</v>
       </c>
-      <c r="F1130" s="143">
+      <c r="F1130" s="140">
         <f>'Template Format ANALISIS I'!F129</f>
         <v>42872.5</v>
       </c>
@@ -27045,7 +27049,7 @@
       <c r="E1137" s="11">
         <v>187.4768</v>
       </c>
-      <c r="F1137" s="143">
+      <c r="F1137" s="140">
         <f>'Template Format ANALISIS I'!F140</f>
         <v>52910</v>
       </c>
@@ -27245,7 +27249,7 @@
       <c r="E1146" s="11">
         <v>497.65780000000007</v>
       </c>
-      <c r="F1146" s="143">
+      <c r="F1146" s="140">
         <f>'Template Format ANALISIS I'!F81</f>
         <v>46475</v>
       </c>
@@ -27445,7 +27449,7 @@
       <c r="E1155" s="11">
         <v>32.520000000000003</v>
       </c>
-      <c r="F1155" s="114">
+      <c r="F1155" s="111">
         <f>'Template Format ANALISIS I'!F366 - 55368</f>
         <v>249057</v>
       </c>
@@ -27649,7 +27653,7 @@
       <c r="E1165" s="35">
         <v>194.3</v>
       </c>
-      <c r="F1165" s="113">
+      <c r="F1165" s="110">
         <f>'Template Format ANALISIS I'!F334 - 291381</f>
         <v>293104</v>
       </c>
@@ -27900,7 +27904,7 @@
       <c r="E1174" s="35">
         <v>15</v>
       </c>
-      <c r="F1174" s="113">
+      <c r="F1174" s="110">
         <f>'Template Format ANALISIS I'!F345 - 66973</f>
         <v>249057</v>
       </c>
@@ -28140,14 +28144,14 @@
       <c r="E1183" s="11">
         <v>31.26</v>
       </c>
-      <c r="F1183" s="114">
+      <c r="F1183" s="111">
         <v>120000</v>
       </c>
       <c r="G1183" s="36">
         <f>F1183*E1183</f>
         <v>3751200</v>
       </c>
-      <c r="I1183" s="125">
+      <c r="I1183" s="122">
         <v>5</v>
       </c>
       <c r="J1183" s="13" t="s">
@@ -28156,7 +28160,7 @@
       <c r="K1183" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1183" s="124">
+      <c r="L1183" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -28185,7 +28189,7 @@
       <c r="E1186" s="11">
         <v>29.137500000000003</v>
       </c>
-      <c r="F1186" s="142">
+      <c r="F1186" s="139">
         <f>'Template Format ANALISIS I'!F70</f>
         <v>95005.35</v>
       </c>
@@ -28218,7 +28222,7 @@
       <c r="B1187" s="38"/>
       <c r="C1187" s="32"/>
       <c r="D1187" s="34"/>
-      <c r="F1187" s="142"/>
+      <c r="F1187" s="139"/>
       <c r="G1187" s="36"/>
       <c r="I1187" s="37">
         <f>'Template Format ANALISIS I'!B64</f>
@@ -28245,7 +28249,7 @@
       <c r="B1188" s="38"/>
       <c r="C1188" s="32"/>
       <c r="D1188" s="34"/>
-      <c r="F1188" s="142"/>
+      <c r="F1188" s="139"/>
       <c r="G1188" s="36"/>
       <c r="I1188" s="37">
         <f>'Template Format ANALISIS I'!B65</f>
@@ -28272,7 +28276,7 @@
       <c r="B1189" s="38"/>
       <c r="C1189" s="32"/>
       <c r="D1189" s="34"/>
-      <c r="F1189" s="142"/>
+      <c r="F1189" s="139"/>
       <c r="G1189" s="36"/>
       <c r="I1189" s="37">
         <f>'Template Format ANALISIS I'!B66</f>
@@ -28299,7 +28303,7 @@
       <c r="B1190" s="38"/>
       <c r="C1190" s="32"/>
       <c r="D1190" s="34"/>
-      <c r="F1190" s="142"/>
+      <c r="F1190" s="139"/>
       <c r="G1190" s="36"/>
       <c r="I1190" s="37">
         <f>'Template Format ANALISIS I'!B67</f>
@@ -28326,7 +28330,7 @@
       <c r="B1191" s="38"/>
       <c r="C1191" s="32"/>
       <c r="D1191" s="34"/>
-      <c r="F1191" s="142"/>
+      <c r="F1191" s="139"/>
       <c r="G1191" s="36"/>
       <c r="I1191" s="37">
         <f>'Template Format ANALISIS I'!B68</f>
@@ -28353,7 +28357,7 @@
       <c r="B1192" s="38"/>
       <c r="C1192" s="32"/>
       <c r="D1192" s="34"/>
-      <c r="F1192" s="142"/>
+      <c r="F1192" s="139"/>
       <c r="G1192" s="36"/>
       <c r="I1192" s="37"/>
       <c r="J1192" s="37"/>
@@ -28371,7 +28375,7 @@
       <c r="B1193" s="38"/>
       <c r="C1193" s="32"/>
       <c r="D1193" s="34"/>
-      <c r="F1193" s="142"/>
+      <c r="F1193" s="139"/>
       <c r="G1193" s="36"/>
       <c r="I1193" s="37"/>
       <c r="J1193" s="37"/>
@@ -28392,7 +28396,7 @@
       <c r="E1194" s="35">
         <v>34.700000000000003</v>
       </c>
-      <c r="F1194" s="113">
+      <c r="F1194" s="110">
         <f>'Template Format ANALISIS I'!F355 - 26939</f>
         <v>43857</v>
       </c>
@@ -28401,15 +28405,15 @@
         <v>1521837.9000000001</v>
       </c>
       <c r="H1194" s="32"/>
-      <c r="I1194" s="134">
+      <c r="I1194" s="131">
         <f>'Template Format ANALISIS I'!B348</f>
         <v>0.12</v>
       </c>
-      <c r="J1194" s="134" t="str">
+      <c r="J1194" s="131" t="str">
         <f>'Template Format ANALISIS I'!C348</f>
         <v>OH</v>
       </c>
-      <c r="K1194" s="134" t="str">
+      <c r="K1194" s="131" t="str">
         <f>'Template Format ANALISIS I'!D348</f>
         <v xml:space="preserve">Pekerja </v>
       </c>
@@ -28430,15 +28434,15 @@
       <c r="F1195" s="80"/>
       <c r="G1195" s="36"/>
       <c r="H1195" s="32"/>
-      <c r="I1195" s="134">
+      <c r="I1195" s="131">
         <f>'Template Format ANALISIS I'!B349</f>
         <v>1.2E-2</v>
       </c>
-      <c r="J1195" s="134" t="str">
+      <c r="J1195" s="131" t="str">
         <f>'Template Format ANALISIS I'!C349</f>
         <v>OH</v>
       </c>
-      <c r="K1195" s="134" t="str">
+      <c r="K1195" s="131" t="str">
         <f>'Template Format ANALISIS I'!D349</f>
         <v>Mandor</v>
       </c>
@@ -28459,15 +28463,15 @@
       <c r="F1196" s="80"/>
       <c r="G1196" s="36"/>
       <c r="H1196" s="32"/>
-      <c r="I1196" s="134">
+      <c r="I1196" s="131">
         <f>'Template Format ANALISIS I'!B350</f>
         <v>0.18</v>
       </c>
-      <c r="J1196" s="134" t="str">
+      <c r="J1196" s="131" t="str">
         <f>'Template Format ANALISIS I'!C350</f>
         <v>OH</v>
       </c>
-      <c r="K1196" s="134" t="str">
+      <c r="K1196" s="131" t="str">
         <f>'Template Format ANALISIS I'!D350</f>
         <v>Tukang</v>
       </c>
@@ -28488,15 +28492,15 @@
       <c r="F1197" s="80"/>
       <c r="G1197" s="36"/>
       <c r="H1197" s="32"/>
-      <c r="I1197" s="134">
+      <c r="I1197" s="131">
         <f>'Template Format ANALISIS I'!B351</f>
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J1197" s="134" t="str">
+      <c r="J1197" s="131" t="str">
         <f>'Template Format ANALISIS I'!C351</f>
         <v>OH</v>
       </c>
-      <c r="K1197" s="134" t="str">
+      <c r="K1197" s="131" t="str">
         <f>'Template Format ANALISIS I'!D351</f>
         <v>Kepala Tukang</v>
       </c>
@@ -28517,15 +28521,15 @@
       <c r="F1198" s="80"/>
       <c r="G1198" s="36"/>
       <c r="H1198" s="32"/>
-      <c r="I1198" s="134">
+      <c r="I1198" s="131">
         <f>'Template Format ANALISIS I'!B352</f>
         <v>1.05</v>
       </c>
-      <c r="J1198" s="134" t="str">
+      <c r="J1198" s="131" t="str">
         <f>'Template Format ANALISIS I'!C352</f>
         <v>M1</v>
       </c>
-      <c r="K1198" s="134" t="str">
+      <c r="K1198" s="131" t="str">
         <f>'Template Format ANALISIS I'!D352</f>
         <v>Gypsum Profil</v>
       </c>
@@ -28546,15 +28550,15 @@
       <c r="F1199" s="80"/>
       <c r="G1199" s="36"/>
       <c r="H1199" s="32"/>
-      <c r="I1199" s="134">
+      <c r="I1199" s="131">
         <f>'Template Format ANALISIS I'!B353</f>
         <v>0.01</v>
       </c>
-      <c r="J1199" s="134" t="str">
+      <c r="J1199" s="131" t="str">
         <f>'Template Format ANALISIS I'!C353</f>
         <v xml:space="preserve">Doz </v>
       </c>
-      <c r="K1199" s="134" t="str">
+      <c r="K1199" s="131" t="str">
         <f>'Template Format ANALISIS I'!D353</f>
         <v>Paku/sekrup</v>
       </c>
@@ -28575,9 +28579,9 @@
       <c r="F1200" s="80"/>
       <c r="G1200" s="36"/>
       <c r="H1200" s="32"/>
-      <c r="I1200" s="134"/>
-      <c r="J1200" s="134"/>
-      <c r="K1200" s="134" t="str">
+      <c r="I1200" s="131"/>
+      <c r="J1200" s="131"/>
+      <c r="K1200" s="131" t="str">
         <f>'Template Format ANALISIS I'!D354</f>
         <v>B.U &amp; Kentungan (10%)</v>
       </c>
@@ -28591,7 +28595,7 @@
       <c r="B1201" s="38"/>
       <c r="C1201" s="32"/>
       <c r="D1201" s="34"/>
-      <c r="F1201" s="142"/>
+      <c r="F1201" s="139"/>
       <c r="G1201" s="36"/>
       <c r="I1201" s="37"/>
       <c r="J1201" s="37"/>
@@ -28829,7 +28833,7 @@
       <c r="E1213" s="11">
         <v>15</v>
       </c>
-      <c r="F1213" s="113">
+      <c r="F1213" s="110">
         <f>'Template Format ANALISIS I'!F239</f>
         <v>4914855</v>
       </c>
@@ -28837,7 +28841,7 @@
         <f>F1213*E1213</f>
         <v>73722825</v>
       </c>
-      <c r="I1213" s="134">
+      <c r="I1213" s="131">
         <f>'Template Format ANALISIS I'!B232</f>
         <v>0.5</v>
       </c>
@@ -28861,7 +28865,7 @@
     <row r="1214" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1214" s="80"/>
       <c r="H1214" s="6"/>
-      <c r="I1214" s="134">
+      <c r="I1214" s="131">
         <f>'Template Format ANALISIS I'!B233</f>
         <v>0.5</v>
       </c>
@@ -28885,7 +28889,7 @@
     <row r="1215" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1215" s="80"/>
       <c r="H1215" s="6"/>
-      <c r="I1215" s="134">
+      <c r="I1215" s="131">
         <f>'Template Format ANALISIS I'!B234</f>
         <v>15</v>
       </c>
@@ -28909,7 +28913,7 @@
     <row r="1216" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1216" s="80"/>
       <c r="H1216" s="6"/>
-      <c r="I1216" s="134">
+      <c r="I1216" s="131">
         <f>'Template Format ANALISIS I'!B235</f>
         <v>0.2</v>
       </c>
@@ -28933,7 +28937,7 @@
     <row r="1217" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1217" s="80"/>
       <c r="H1217" s="6"/>
-      <c r="I1217" s="134">
+      <c r="I1217" s="131">
         <f>'Template Format ANALISIS I'!B236</f>
         <v>15</v>
       </c>
@@ -28957,7 +28961,7 @@
     <row r="1218" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1218" s="80"/>
       <c r="H1218" s="6"/>
-      <c r="I1218" s="134">
+      <c r="I1218" s="131">
         <f>'Template Format ANALISIS I'!B237</f>
         <v>0.2</v>
       </c>
@@ -28999,7 +29003,7 @@
       <c r="E1220" s="11">
         <v>15</v>
       </c>
-      <c r="F1220" s="113">
+      <c r="F1220" s="110">
         <f>'Template Format ANALISIS I'!F249</f>
         <v>696300</v>
       </c>
@@ -29007,7 +29011,7 @@
         <f>F1220*E1220</f>
         <v>10444500</v>
       </c>
-      <c r="I1220" s="134">
+      <c r="I1220" s="131">
         <f>'Template Format ANALISIS I'!B242</f>
         <v>0.5</v>
       </c>
@@ -29030,7 +29034,7 @@
     </row>
     <row r="1221" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1221" s="80"/>
-      <c r="I1221" s="134">
+      <c r="I1221" s="131">
         <f>'Template Format ANALISIS I'!B243</f>
         <v>0.5</v>
       </c>
@@ -29053,7 +29057,7 @@
     </row>
     <row r="1222" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1222" s="80"/>
-      <c r="I1222" s="134">
+      <c r="I1222" s="131">
         <f>'Template Format ANALISIS I'!B244</f>
         <v>15</v>
       </c>
@@ -29076,7 +29080,7 @@
     </row>
     <row r="1223" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1223" s="80"/>
-      <c r="I1223" s="134">
+      <c r="I1223" s="131">
         <f>'Template Format ANALISIS I'!B245</f>
         <v>0.2</v>
       </c>
@@ -29099,7 +29103,7 @@
     </row>
     <row r="1224" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1224" s="80"/>
-      <c r="I1224" s="134">
+      <c r="I1224" s="131">
         <f>'Template Format ANALISIS I'!B246</f>
         <v>15</v>
       </c>
@@ -29122,7 +29126,7 @@
     </row>
     <row r="1225" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1225" s="80"/>
-      <c r="I1225" s="134">
+      <c r="I1225" s="131">
         <f>'Template Format ANALISIS I'!B247</f>
         <v>0.2</v>
       </c>
@@ -29168,7 +29172,7 @@
       <c r="E1228" s="11">
         <v>6</v>
       </c>
-      <c r="F1228" s="143">
+      <c r="F1228" s="140">
         <f>'Template Format ANALISIS I'!F150</f>
         <v>52707.6</v>
       </c>
@@ -29508,7 +29512,7 @@
       <c r="E1244" s="11">
         <v>5</v>
       </c>
-      <c r="F1244" s="143">
+      <c r="F1244" s="140">
         <f>'Template Format ANALISIS I'!F170</f>
         <v>253376.2</v>
       </c>
@@ -29540,7 +29544,7 @@
     <row r="1245" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C1245" s="54"/>
       <c r="D1245" s="52"/>
-      <c r="F1245" s="143"/>
+      <c r="F1245" s="140"/>
       <c r="I1245" s="62">
         <f>'Template Format ANALISIS I'!B164</f>
         <v>4.1000000000000003E-3</v>
@@ -29565,7 +29569,7 @@
     <row r="1246" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C1246" s="54"/>
       <c r="D1246" s="52"/>
-      <c r="F1246" s="143"/>
+      <c r="F1246" s="140"/>
       <c r="I1246" s="62">
         <f>'Template Format ANALISIS I'!B165</f>
         <v>0.13500000000000001</v>
@@ -29590,7 +29594,7 @@
     <row r="1247" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C1247" s="54"/>
       <c r="D1247" s="52"/>
-      <c r="F1247" s="143"/>
+      <c r="F1247" s="140"/>
       <c r="I1247" s="62">
         <f>'Template Format ANALISIS I'!B166</f>
         <v>1.35E-2</v>
@@ -29615,7 +29619,7 @@
     <row r="1248" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C1248" s="54"/>
       <c r="D1248" s="52"/>
-      <c r="F1248" s="143"/>
+      <c r="F1248" s="140"/>
       <c r="I1248" s="62">
         <f>'Template Format ANALISIS I'!B167</f>
         <v>1.2</v>
@@ -29640,7 +29644,7 @@
     <row r="1249" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C1249" s="54"/>
       <c r="D1249" s="52"/>
-      <c r="F1249" s="143"/>
+      <c r="F1249" s="140"/>
       <c r="I1249" s="62">
         <f>'Template Format ANALISIS I'!B168</f>
         <v>1</v>
@@ -29662,7 +29666,7 @@
     <row r="1250" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C1250" s="54"/>
       <c r="D1250" s="52"/>
-      <c r="F1250" s="143"/>
+      <c r="F1250" s="140"/>
       <c r="I1250" s="62"/>
       <c r="J1250" s="62"/>
       <c r="K1250" s="62" t="str">
@@ -29678,7 +29682,7 @@
     <row r="1251" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C1251" s="54"/>
       <c r="D1251" s="52"/>
-      <c r="F1251" s="143"/>
+      <c r="F1251" s="140"/>
       <c r="I1251" s="62"/>
     </row>
     <row r="1252" spans="2:13" x14ac:dyDescent="0.3">
@@ -29873,7 +29877,7 @@
       <c r="E1260" s="57">
         <v>3</v>
       </c>
-      <c r="F1260" s="135">
+      <c r="F1260" s="132">
         <f>'Template Format ANALISIS I'!F376 - 132266</f>
         <v>40535.200000000012</v>
       </c>
@@ -29882,15 +29886,15 @@
         <v>121605.60000000003</v>
       </c>
       <c r="H1260" s="59"/>
-      <c r="I1260" s="138">
+      <c r="I1260" s="135">
         <f>'Template Format ANALISIS I'!B369</f>
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="J1260" s="138" t="str">
+      <c r="J1260" s="135" t="str">
         <f>'Template Format ANALISIS I'!C369</f>
         <v>OH</v>
       </c>
-      <c r="K1260" s="138" t="str">
+      <c r="K1260" s="135" t="str">
         <f>'Template Format ANALISIS I'!D369</f>
         <v xml:space="preserve">Pekerja </v>
       </c>
@@ -29909,15 +29913,15 @@
       <c r="F1261" s="76"/>
       <c r="G1261" s="51"/>
       <c r="H1261" s="59"/>
-      <c r="I1261" s="138">
+      <c r="I1261" s="135">
         <f>'Template Format ANALISIS I'!B370</f>
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="J1261" s="138" t="str">
+      <c r="J1261" s="135" t="str">
         <f>'Template Format ANALISIS I'!C370</f>
         <v>OH</v>
       </c>
-      <c r="K1261" s="138" t="str">
+      <c r="K1261" s="135" t="str">
         <f>'Template Format ANALISIS I'!D370</f>
         <v>Mandor</v>
       </c>
@@ -29936,15 +29940,15 @@
       <c r="F1262" s="76"/>
       <c r="G1262" s="51"/>
       <c r="H1262" s="59"/>
-      <c r="I1262" s="138">
+      <c r="I1262" s="135">
         <f>'Template Format ANALISIS I'!B371</f>
         <v>0.13500000000000001</v>
       </c>
-      <c r="J1262" s="138" t="str">
+      <c r="J1262" s="135" t="str">
         <f>'Template Format ANALISIS I'!C371</f>
         <v>OH</v>
       </c>
-      <c r="K1262" s="138" t="str">
+      <c r="K1262" s="135" t="str">
         <f>'Template Format ANALISIS I'!D371</f>
         <v xml:space="preserve">Tukang </v>
       </c>
@@ -29963,15 +29967,15 @@
       <c r="F1263" s="76"/>
       <c r="G1263" s="51"/>
       <c r="H1263" s="59"/>
-      <c r="I1263" s="138">
+      <c r="I1263" s="135">
         <f>'Template Format ANALISIS I'!B372</f>
         <v>1.35E-2</v>
       </c>
-      <c r="J1263" s="138" t="str">
+      <c r="J1263" s="135" t="str">
         <f>'Template Format ANALISIS I'!C372</f>
         <v>OH</v>
       </c>
-      <c r="K1263" s="138" t="str">
+      <c r="K1263" s="135" t="str">
         <f>'Template Format ANALISIS I'!D372</f>
         <v>Kepala Tukang</v>
       </c>
@@ -29990,15 +29994,15 @@
       <c r="F1264" s="76"/>
       <c r="G1264" s="51"/>
       <c r="H1264" s="59"/>
-      <c r="I1264" s="138">
+      <c r="I1264" s="135">
         <f>'Template Format ANALISIS I'!B373</f>
         <v>1</v>
       </c>
-      <c r="J1264" s="138" t="str">
+      <c r="J1264" s="135" t="str">
         <f>'Template Format ANALISIS I'!C373</f>
         <v>Bh</v>
       </c>
-      <c r="K1264" s="138" t="str">
+      <c r="K1264" s="135" t="str">
         <f>'Template Format ANALISIS I'!D373</f>
         <v>Floordrain Besi</v>
       </c>
@@ -30017,12 +30021,12 @@
       <c r="F1265" s="76"/>
       <c r="G1265" s="51"/>
       <c r="H1265" s="59"/>
-      <c r="I1265" s="138">
+      <c r="I1265" s="135">
         <f>'Template Format ANALISIS I'!B374</f>
         <v>1</v>
       </c>
-      <c r="J1265" s="138"/>
-      <c r="K1265" s="138" t="str">
+      <c r="J1265" s="135"/>
+      <c r="K1265" s="135" t="str">
         <f>'Template Format ANALISIS I'!D374</f>
         <v>Perlengkapan</v>
       </c>
@@ -30041,9 +30045,9 @@
       <c r="F1266" s="76"/>
       <c r="G1266" s="51"/>
       <c r="H1266" s="59"/>
-      <c r="I1266" s="138"/>
-      <c r="J1266" s="138"/>
-      <c r="K1266" s="138" t="str">
+      <c r="I1266" s="135"/>
+      <c r="J1266" s="135"/>
+      <c r="K1266" s="135" t="str">
         <f>'Template Format ANALISIS I'!D375</f>
         <v>B.U &amp; Kentungan (10%)</v>
       </c>
@@ -30092,7 +30096,7 @@
       <c r="E1270" s="11">
         <v>13.32</v>
       </c>
-      <c r="F1270" s="115">
+      <c r="F1270" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -30221,7 +30225,7 @@
       <c r="E1276" s="11">
         <v>3328.51</v>
       </c>
-      <c r="F1276" s="115">
+      <c r="F1276" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -30374,8 +30378,8 @@
       <c r="B1282" s="71"/>
       <c r="C1282" s="10"/>
       <c r="I1282" s="26"/>
-      <c r="J1282" s="118"/>
-      <c r="K1282" s="118"/>
+      <c r="J1282" s="115"/>
+      <c r="K1282" s="115"/>
       <c r="L1282" s="74"/>
       <c r="M1282" s="44"/>
     </row>
@@ -30392,7 +30396,7 @@
       <c r="E1283" s="11">
         <v>122.1</v>
       </c>
-      <c r="F1283" s="115">
+      <c r="F1283" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -30600,7 +30604,7 @@
       <c r="E1293" s="11">
         <v>6.03</v>
       </c>
-      <c r="F1293" s="115">
+      <c r="F1293" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -30729,7 +30733,7 @@
       <c r="E1299" s="11">
         <v>1207.5999999999999</v>
       </c>
-      <c r="F1299" s="115">
+      <c r="F1299" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -30882,8 +30886,8 @@
       <c r="B1305" s="71"/>
       <c r="C1305" s="10"/>
       <c r="I1305" s="26"/>
-      <c r="J1305" s="118"/>
-      <c r="K1305" s="118"/>
+      <c r="J1305" s="115"/>
+      <c r="K1305" s="115"/>
       <c r="L1305" s="74"/>
       <c r="M1305" s="44"/>
     </row>
@@ -30900,7 +30904,7 @@
       <c r="E1306" s="11">
         <v>60.26</v>
       </c>
-      <c r="F1306" s="115">
+      <c r="F1306" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -31108,7 +31112,7 @@
       <c r="E1316" s="11">
         <v>4.49</v>
       </c>
-      <c r="F1316" s="115">
+      <c r="F1316" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -31237,7 +31241,7 @@
       <c r="E1322" s="11">
         <v>1543.07</v>
       </c>
-      <c r="F1322" s="115">
+      <c r="F1322" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -31390,8 +31394,8 @@
       <c r="B1328" s="71"/>
       <c r="C1328" s="10"/>
       <c r="I1328" s="26"/>
-      <c r="J1328" s="118"/>
-      <c r="K1328" s="118"/>
+      <c r="J1328" s="115"/>
+      <c r="K1328" s="115"/>
       <c r="L1328" s="74"/>
       <c r="M1328" s="44"/>
     </row>
@@ -31408,7 +31412,7 @@
       <c r="E1329" s="11">
         <v>80.61</v>
       </c>
-      <c r="F1329" s="115">
+      <c r="F1329" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -31616,7 +31620,7 @@
       <c r="E1339" s="11">
         <v>39.479999999999997</v>
       </c>
-      <c r="F1339" s="115">
+      <c r="F1339" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -31750,14 +31754,14 @@
       <c r="E1345" s="11">
         <v>328.97</v>
       </c>
-      <c r="F1345" s="114">
+      <c r="F1345" s="111">
         <v>220000</v>
       </c>
       <c r="G1345" s="12">
         <f>F1345*E1345</f>
         <v>72373400</v>
       </c>
-      <c r="I1345" s="116">
+      <c r="I1345" s="113">
         <v>0.5</v>
       </c>
       <c r="J1345" s="13" t="s">
@@ -31766,7 +31770,7 @@
       <c r="K1345" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1345" s="124">
+      <c r="L1345" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -31787,14 +31791,14 @@
       <c r="E1347" s="11">
         <v>328.97</v>
       </c>
-      <c r="F1347" s="114">
+      <c r="F1347" s="111">
         <v>240000</v>
       </c>
       <c r="G1347" s="12">
         <f>F1347*E1347</f>
         <v>78952800</v>
       </c>
-      <c r="I1347" s="116">
+      <c r="I1347" s="113">
         <v>0.5</v>
       </c>
       <c r="J1347" s="13" t="s">
@@ -31803,7 +31807,7 @@
       <c r="K1347" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1347" s="124">
+      <c r="L1347" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -31826,7 +31830,7 @@
       <c r="E1349" s="11">
         <v>328.97</v>
       </c>
-      <c r="F1349" s="115">
+      <c r="F1349" s="112">
         <f>'Template Format ANALISIS I'!F289 + 132312</f>
         <v>434247</v>
       </c>
@@ -32039,7 +32043,7 @@
       <c r="E1359" s="11">
         <v>0.48</v>
       </c>
-      <c r="F1359" s="115">
+      <c r="F1359" s="112">
         <f>'Template Format ANALISIS I'!F263 - 396730</f>
         <v>1288635</v>
       </c>
@@ -32167,7 +32171,7 @@
       <c r="E1365" s="11">
         <v>131.97999999999999</v>
       </c>
-      <c r="F1365" s="115">
+      <c r="F1365" s="112">
         <f>'Template Format ANALISIS I'!F275 - 3225.2</f>
         <v>17313.3</v>
       </c>
@@ -32326,7 +32330,7 @@
       <c r="E1372" s="11">
         <v>13.2</v>
       </c>
-      <c r="F1372" s="115">
+      <c r="F1372" s="112">
         <f>'Template Format ANALISIS I'!F289 + 196112</f>
         <v>498047</v>
       </c>
@@ -32356,7 +32360,7 @@
       </c>
     </row>
     <row r="1373" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F1373" s="118"/>
+      <c r="F1373" s="115"/>
       <c r="I1373" s="26">
         <f>'Template Format ANALISIS I'!B281</f>
         <v>1.1000000000000001E-2</v>
@@ -32379,7 +32383,7 @@
       </c>
     </row>
     <row r="1374" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F1374" s="118"/>
+      <c r="F1374" s="115"/>
       <c r="I1374" s="26">
         <f>'Template Format ANALISIS I'!B282</f>
         <v>0.16500000000000001</v>
@@ -32402,7 +32406,7 @@
       </c>
     </row>
     <row r="1375" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F1375" s="118"/>
+      <c r="F1375" s="115"/>
       <c r="I1375" s="26">
         <f>'Template Format ANALISIS I'!B283</f>
         <v>8.2500000000000004E-3</v>
@@ -32425,7 +32429,7 @@
       </c>
     </row>
     <row r="1376" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F1376" s="118"/>
+      <c r="F1376" s="115"/>
       <c r="I1376" s="26">
         <f>'Template Format ANALISIS I'!B285</f>
         <v>0.04</v>
@@ -32448,7 +32452,7 @@
       </c>
     </row>
     <row r="1377" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F1377" s="118"/>
+      <c r="F1377" s="115"/>
       <c r="I1377" s="26">
         <f>'Template Format ANALISIS I'!B286</f>
         <v>0.3</v>
@@ -32471,7 +32475,7 @@
       </c>
     </row>
     <row r="1378" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F1378" s="118"/>
+      <c r="F1378" s="115"/>
       <c r="I1378" s="26">
         <f>'Template Format ANALISIS I'!B287</f>
         <v>0.1</v>
@@ -32494,7 +32498,7 @@
       </c>
     </row>
     <row r="1379" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F1379" s="118"/>
+      <c r="F1379" s="115"/>
       <c r="I1379" s="26">
         <f>'Template Format ANALISIS I'!B288</f>
         <v>0.82</v>
@@ -32517,7 +32521,7 @@
       </c>
     </row>
     <row r="1380" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F1380" s="118"/>
+      <c r="F1380" s="115"/>
       <c r="I1380" s="26"/>
       <c r="J1380" s="26"/>
       <c r="K1380" s="26"/>
@@ -32537,14 +32541,14 @@
       <c r="E1381" s="11">
         <v>342.57</v>
       </c>
-      <c r="F1381" s="114">
+      <c r="F1381" s="111">
         <v>148753</v>
       </c>
       <c r="G1381" s="36">
         <f>F1381*E1381</f>
         <v>50958315.210000001</v>
       </c>
-      <c r="I1381" s="125">
+      <c r="I1381" s="122">
         <v>5</v>
       </c>
       <c r="J1381" s="13" t="s">
@@ -32553,7 +32557,7 @@
       <c r="K1381" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1381" s="124">
+      <c r="L1381" s="121">
         <v>110000</v>
       </c>
       <c r="M1381" s="44"/>
@@ -32562,7 +32566,7 @@
       <c r="F1382" s="74"/>
       <c r="G1382" s="36"/>
       <c r="H1382" s="6"/>
-      <c r="I1382" s="134"/>
+      <c r="I1382" s="131"/>
       <c r="J1382" s="7"/>
       <c r="K1382" s="7"/>
       <c r="M1382" s="44"/>
@@ -32580,7 +32584,7 @@
       <c r="E1383" s="11">
         <v>82</v>
       </c>
-      <c r="F1383" s="142">
+      <c r="F1383" s="139">
         <f>'Template Format ANALISIS I'!F120</f>
         <v>77396</v>
       </c>
@@ -32753,7 +32757,7 @@
       <c r="E1391" s="11">
         <v>82</v>
       </c>
-      <c r="F1391" s="143">
+      <c r="F1391" s="140">
         <f>'Template Format ANALISIS I'!F129</f>
         <v>42872.5</v>
       </c>
@@ -32903,7 +32907,7 @@
       <c r="E1398" s="11">
         <v>41</v>
       </c>
-      <c r="F1398" s="143">
+      <c r="F1398" s="140">
         <f>'Template Format ANALISIS I'!F140</f>
         <v>52910</v>
       </c>
@@ -33099,7 +33103,7 @@
       <c r="E1407" s="11">
         <v>41</v>
       </c>
-      <c r="F1407" s="143">
+      <c r="F1407" s="140">
         <f>'Template Format ANALISIS I'!F81</f>
         <v>46475</v>
       </c>
@@ -33299,14 +33303,14 @@
       <c r="E1416" s="11">
         <v>373.42</v>
       </c>
-      <c r="F1416" s="114">
+      <c r="F1416" s="111">
         <v>120000</v>
       </c>
       <c r="G1416" s="36">
         <f>F1416*E1416</f>
         <v>44810400</v>
       </c>
-      <c r="I1416" s="125">
+      <c r="I1416" s="122">
         <v>5</v>
       </c>
       <c r="J1416" s="13" t="s">
@@ -33315,7 +33319,7 @@
       <c r="K1416" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1416" s="124">
+      <c r="L1416" s="121">
         <v>110000</v>
       </c>
       <c r="M1416" s="44"/>
@@ -33323,7 +33327,7 @@
     <row r="1417" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F1417" s="74"/>
       <c r="G1417" s="36"/>
-      <c r="I1417" s="134"/>
+      <c r="I1417" s="131"/>
       <c r="J1417" s="7"/>
       <c r="K1417" s="7"/>
       <c r="M1417" s="44"/>
@@ -33729,14 +33733,14 @@
       <c r="E1438" s="11">
         <v>1</v>
       </c>
-      <c r="F1438" s="114">
+      <c r="F1438" s="111">
         <v>40000000</v>
       </c>
       <c r="G1438" s="36">
         <f>F1438*E1438</f>
         <v>40000000</v>
       </c>
-      <c r="I1438" s="116">
+      <c r="I1438" s="113">
         <v>0.5</v>
       </c>
       <c r="J1438" s="13" t="s">
@@ -33745,7 +33749,7 @@
       <c r="K1438" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1438" s="124">
+      <c r="L1438" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -33773,14 +33777,14 @@
       <c r="E1441" s="11">
         <v>1</v>
       </c>
-      <c r="F1441" s="114">
+      <c r="F1441" s="111">
         <v>5000000</v>
       </c>
       <c r="G1441" s="36">
         <f>F1441*E1441</f>
         <v>5000000</v>
       </c>
-      <c r="I1441" s="116">
+      <c r="I1441" s="113">
         <v>0.5</v>
       </c>
       <c r="J1441" s="13" t="s">
@@ -33789,7 +33793,7 @@
       <c r="K1441" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1441" s="124">
+      <c r="L1441" s="121">
         <v>110000</v>
       </c>
     </row>
@@ -35209,7 +35213,7 @@
       <c r="D105" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E105" s="120">
+      <c r="E105" s="117">
         <v>2485000</v>
       </c>
       <c r="F105" s="44">
@@ -35227,7 +35231,7 @@
       <c r="D106" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="E106" s="120">
+      <c r="E106" s="117">
         <v>18000</v>
       </c>
       <c r="F106" s="44">
@@ -35245,7 +35249,7 @@
       <c r="D107" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E107" s="120">
+      <c r="E107" s="117">
         <v>10000</v>
       </c>
       <c r="F107" s="44">
@@ -35263,7 +35267,7 @@
       <c r="D108" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="E108" s="120">
+      <c r="E108" s="117">
         <v>180500</v>
       </c>
       <c r="F108" s="44">
@@ -35281,7 +35285,7 @@
       <c r="D109" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="E109" s="120">
+      <c r="E109" s="117">
         <v>15000</v>
       </c>
       <c r="F109" s="44">
@@ -35801,7 +35805,7 @@
       <c r="D147" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="E147" s="120">
+      <c r="E147" s="117">
         <v>27000</v>
       </c>
       <c r="F147" s="44">
@@ -35816,7 +35820,7 @@
       <c r="D148" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="E148" s="120">
+      <c r="E148" s="117">
         <v>2700</v>
       </c>
       <c r="F148" s="44">
@@ -36558,7 +36562,7 @@
       <c r="D205" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E205" s="121">
+      <c r="E205" s="118">
         <f>+E192</f>
         <v>130000</v>
       </c>
@@ -37263,7 +37267,7 @@
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B260" s="122">
+      <c r="B260" s="119">
         <v>1</v>
       </c>
       <c r="C260" s="38" t="s">
@@ -38507,143 +38511,143 @@
       <c r="A347" s="1">
         <v>34</v>
       </c>
-      <c r="B347" s="133" t="s">
+      <c r="B347" s="130" t="s">
         <v>214</v>
       </c>
-      <c r="C347" s="126"/>
-      <c r="D347" s="126"/>
-      <c r="E347" s="129"/>
-      <c r="F347" s="129"/>
+      <c r="C347" s="123"/>
+      <c r="D347" s="123"/>
+      <c r="E347" s="126"/>
+      <c r="F347" s="126"/>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B348" s="130">
+      <c r="B348" s="127">
         <v>0.12</v>
       </c>
-      <c r="C348" s="131" t="s">
+      <c r="C348" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="D348" s="131" t="s">
+      <c r="D348" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="E348" s="129">
+      <c r="E348" s="126">
         <v>110000</v>
       </c>
-      <c r="F348" s="127">
+      <c r="F348" s="124">
         <f>B348*E348</f>
         <v>13200</v>
       </c>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B349" s="130">
+      <c r="B349" s="127">
         <f>+B348*0.1</f>
         <v>1.2E-2</v>
       </c>
-      <c r="C349" s="131" t="s">
+      <c r="C349" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="D349" s="131" t="s">
+      <c r="D349" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="E349" s="129">
+      <c r="E349" s="126">
         <v>120000</v>
       </c>
-      <c r="F349" s="127">
+      <c r="F349" s="124">
         <f t="shared" ref="F349:F353" si="31">B349*E349</f>
         <v>1440</v>
       </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B350" s="132">
+      <c r="B350" s="129">
         <v>0.18</v>
       </c>
-      <c r="C350" s="131" t="s">
+      <c r="C350" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="D350" s="131" t="s">
+      <c r="D350" s="128" t="s">
         <v>145</v>
       </c>
-      <c r="E350" s="129">
+      <c r="E350" s="126">
         <v>130000</v>
       </c>
-      <c r="F350" s="127">
+      <c r="F350" s="124">
         <f t="shared" si="31"/>
         <v>23400</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B351" s="132">
+      <c r="B351" s="129">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C351" s="131" t="s">
+      <c r="C351" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="D351" s="131" t="s">
+      <c r="D351" s="128" t="s">
         <v>24</v>
       </c>
-      <c r="E351" s="129">
+      <c r="E351" s="126">
         <v>140000</v>
       </c>
-      <c r="F351" s="127">
+      <c r="F351" s="124">
         <f t="shared" si="31"/>
         <v>2520</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B352" s="132">
+      <c r="B352" s="129">
         <v>1.05</v>
       </c>
-      <c r="C352" s="131" t="s">
+      <c r="C352" s="128" t="s">
         <v>104</v>
       </c>
-      <c r="D352" s="126" t="s">
+      <c r="D352" s="123" t="s">
         <v>215</v>
       </c>
-      <c r="E352" s="129">
+      <c r="E352" s="126">
         <v>22500</v>
       </c>
-      <c r="F352" s="127">
+      <c r="F352" s="124">
         <f t="shared" si="31"/>
         <v>23625</v>
       </c>
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B353" s="132">
+      <c r="B353" s="129">
         <v>0.01</v>
       </c>
-      <c r="C353" s="131" t="s">
+      <c r="C353" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="D353" s="126" t="s">
+      <c r="D353" s="123" t="s">
         <v>69</v>
       </c>
-      <c r="E353" s="129">
+      <c r="E353" s="126">
         <v>17500</v>
       </c>
-      <c r="F353" s="127">
+      <c r="F353" s="124">
         <f t="shared" si="31"/>
         <v>175</v>
       </c>
     </row>
     <row r="354" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B354" s="132"/>
-      <c r="C354" s="126"/>
-      <c r="D354" s="126" t="s">
+      <c r="B354" s="129"/>
+      <c r="C354" s="123"/>
+      <c r="D354" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="E354" s="129"/>
-      <c r="F354" s="127">
+      <c r="E354" s="126"/>
+      <c r="F354" s="124">
         <f>SUM(F348:F353)*10%</f>
         <v>6436</v>
       </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B355" s="132"/>
-      <c r="C355" s="126"/>
-      <c r="D355" s="128" t="s">
+      <c r="B355" s="129"/>
+      <c r="C355" s="123"/>
+      <c r="D355" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="E355" s="129"/>
-      <c r="F355" s="127">
+      <c r="E355" s="126"/>
+      <c r="F355" s="124">
         <f>SUM(F348:F354)</f>
         <v>70796</v>
       </c>
@@ -38669,7 +38673,7 @@
       <c r="E358" s="4">
         <v>110000</v>
       </c>
-      <c r="F358" s="127">
+      <c r="F358" s="124">
         <f>B358*E358</f>
         <v>44000</v>
       </c>
@@ -38687,7 +38691,7 @@
       <c r="E359" s="4">
         <v>120000</v>
       </c>
-      <c r="F359" s="127">
+      <c r="F359" s="124">
         <f t="shared" ref="F359:F364" si="32">B359*E359</f>
         <v>5400</v>
       </c>
@@ -38705,7 +38709,7 @@
       <c r="E360" s="4">
         <v>130000</v>
       </c>
-      <c r="F360" s="127">
+      <c r="F360" s="124">
         <f t="shared" si="32"/>
         <v>58500</v>
       </c>
@@ -38723,7 +38727,7 @@
       <c r="E361" s="4">
         <v>140000</v>
       </c>
-      <c r="F361" s="127">
+      <c r="F361" s="124">
         <f t="shared" si="32"/>
         <v>6300</v>
       </c>
@@ -38741,7 +38745,7 @@
       <c r="E362" s="4">
         <v>145000</v>
       </c>
-      <c r="F362" s="127">
+      <c r="F362" s="124">
         <f t="shared" si="32"/>
         <v>145000</v>
       </c>
@@ -38759,7 +38763,7 @@
       <c r="E363" s="4">
         <v>200000</v>
       </c>
-      <c r="F363" s="127">
+      <c r="F363" s="124">
         <f t="shared" si="32"/>
         <v>3599.9999999999995</v>
       </c>
@@ -38777,25 +38781,25 @@
       <c r="E364" s="4">
         <v>1500</v>
       </c>
-      <c r="F364" s="127">
+      <c r="F364" s="124">
         <f t="shared" si="32"/>
         <v>13950.000000000002</v>
       </c>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D365" s="126" t="s">
+      <c r="D365" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="F365" s="127">
+      <c r="F365" s="124">
         <f>SUM(F358:F364)*10%</f>
         <v>27675</v>
       </c>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D366" s="128" t="s">
+      <c r="D366" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="F366" s="127">
+      <c r="F366" s="124">
         <f>SUM(F358:F365)</f>
         <v>304425</v>
       </c>
@@ -38821,7 +38825,7 @@
       <c r="E369" s="4">
         <v>110000</v>
       </c>
-      <c r="F369" s="127">
+      <c r="F369" s="124">
         <f>B369*E369</f>
         <v>8910</v>
       </c>
@@ -38839,7 +38843,7 @@
       <c r="E370" s="4">
         <v>120000</v>
       </c>
-      <c r="F370" s="127">
+      <c r="F370" s="124">
         <f t="shared" ref="F370:F374" si="33">B370*E370</f>
         <v>492.00000000000006</v>
       </c>
@@ -38857,7 +38861,7 @@
       <c r="E371" s="4">
         <v>130000</v>
       </c>
-      <c r="F371" s="127">
+      <c r="F371" s="124">
         <f t="shared" si="33"/>
         <v>17550</v>
       </c>
@@ -38875,7 +38879,7 @@
       <c r="E372" s="4">
         <v>140000</v>
       </c>
-      <c r="F372" s="127">
+      <c r="F372" s="124">
         <f t="shared" si="33"/>
         <v>1890</v>
       </c>
@@ -38893,7 +38897,7 @@
       <c r="E373" s="4">
         <v>95000</v>
       </c>
-      <c r="F373" s="127">
+      <c r="F373" s="124">
         <f t="shared" si="33"/>
         <v>95000</v>
       </c>
@@ -38908,25 +38912,25 @@
       <c r="E374" s="4">
         <v>33250</v>
       </c>
-      <c r="F374" s="127">
+      <c r="F374" s="124">
         <f t="shared" si="33"/>
         <v>33250</v>
       </c>
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D375" s="126" t="s">
+      <c r="D375" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="F375" s="127">
+      <c r="F375" s="124">
         <f>SUM(F369:F374)*10%</f>
         <v>15709.2</v>
       </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D376" s="128" t="s">
+      <c r="D376" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="F376" s="127">
+      <c r="F376" s="124">
         <f>SUM(F369:F375)</f>
         <v>172801.2</v>
       </c>
@@ -38952,7 +38956,7 @@
       <c r="E379" s="4">
         <v>274200</v>
       </c>
-      <c r="F379" s="127">
+      <c r="F379" s="124">
         <f>B379*E379</f>
         <v>32904</v>
       </c>
@@ -38970,7 +38974,7 @@
       <c r="E380" s="4">
         <v>1056157.5132275133</v>
       </c>
-      <c r="F380" s="127">
+      <c r="F380" s="124">
         <f t="shared" ref="F380:F382" si="34">B380*E380</f>
         <v>253477.80317460318</v>
       </c>
@@ -38988,7 +38992,7 @@
       <c r="E381" s="4">
         <v>138050</v>
       </c>
-      <c r="F381" s="127">
+      <c r="F381" s="124">
         <f t="shared" si="34"/>
         <v>138050</v>
       </c>
@@ -39006,25 +39010,25 @@
       <c r="E382" s="4">
         <v>70560</v>
       </c>
-      <c r="F382" s="127">
+      <c r="F382" s="124">
         <f t="shared" si="34"/>
         <v>70560</v>
       </c>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D383" s="126" t="s">
+      <c r="D383" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="F383" s="127">
+      <c r="F383" s="124">
         <f>SUM(F377:F382)*10%</f>
         <v>49499.180317460319</v>
       </c>
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D384" s="128" t="s">
+      <c r="D384" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="F384" s="127">
+      <c r="F384" s="124">
         <f>SUM(F377:F383)</f>
         <v>544490.98349206347</v>
       </c>

</xml_diff>

<commit_message>
chore: update for biaya RAB dan Aplikasi comparison
</commit_message>
<xml_diff>
--- a/files/template_format.xlsx
+++ b/files/template_format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lunba7th\Documents\S2 - Teknik Sipil\S2 Thesis start from 0\Data\RAB FPIK - Gedung Pendidkan - TA 2018 - BLU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\lunba\Project\ga_civil_construction_resource_optimization\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="264">
   <si>
     <t>PEKERJAAN</t>
   </si>
@@ -809,6 +809,15 @@
   <si>
     <t>TOTAL HARI AKUMULATIF PENGERJAAN PROYEK (PEKERJA)</t>
   </si>
+  <si>
+    <t>ANALISIS III (GA)</t>
+  </si>
+  <si>
+    <t>Biaya RAB</t>
+  </si>
+  <si>
+    <t>Biaya Aplikasi</t>
+  </si>
 </sst>
 </file>
 
@@ -819,7 +828,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$IDR]\ #,##0.00;[Red][$IDR]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$IDR]\ #,##0.00;[Red][$IDR]\ #,##0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1211,7 +1220,7 @@
     <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1332,7 +1341,19 @@
     <xf numFmtId="4" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1349,18 +1370,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1647,11 +1656,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:X1441"/>
+  <dimension ref="B1:AA1441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T21" sqref="T21"/>
+      <selection pane="bottomLeft" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1676,57 +1685,63 @@
     <col min="18" max="18" width="22.88671875" style="13" customWidth="1"/>
     <col min="19" max="19" width="8.88671875" style="13"/>
     <col min="20" max="20" width="17.77734375" style="42" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.88671875" style="1"/>
-    <col min="22" max="22" width="53.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.88671875" style="1"/>
+    <col min="21" max="23" width="17.77734375" style="42" customWidth="1"/>
+    <col min="24" max="24" width="8.88671875" style="1"/>
+    <col min="25" max="25" width="53.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.3">
       <c r="E1" s="3"/>
       <c r="H1" s="6"/>
       <c r="I1" s="26"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B2" s="135"/>
-      <c r="C2" s="134" t="s">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B2" s="139"/>
+      <c r="C2" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="137" t="s">
+      <c r="D2" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="138" t="s">
+      <c r="I2" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="141"/>
+      <c r="M2" s="141"/>
       <c r="N2" s="18"/>
-      <c r="O2" s="137" t="s">
+      <c r="O2" s="141" t="s">
         <v>154</v>
       </c>
-      <c r="P2" s="137"/>
-      <c r="Q2" s="137"/>
-      <c r="R2" s="137"/>
-      <c r="S2" s="137"/>
-      <c r="T2" s="137"/>
-      <c r="V2" s="134" t="s">
+      <c r="P2" s="141"/>
+      <c r="Q2" s="141"/>
+      <c r="R2" s="141"/>
+      <c r="S2" s="141"/>
+      <c r="T2" s="141"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="141" t="s">
+        <v>261</v>
+      </c>
+      <c r="W2" s="141"/>
+      <c r="Y2" s="138" t="s">
         <v>155</v>
       </c>
-      <c r="W2" s="134"/>
-      <c r="X2" s="134"/>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B3" s="136"/>
-      <c r="C3" s="134"/>
+      <c r="Z2" s="138"/>
+      <c r="AA2" s="138"/>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B3" s="140"/>
+      <c r="C3" s="138"/>
       <c r="D3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1759,22 +1774,29 @@
       <c r="O3" s="82" t="s">
         <v>156</v>
       </c>
-      <c r="P3" s="140"/>
+      <c r="P3" s="135"/>
       <c r="Q3" s="24" t="s">
         <v>157</v>
       </c>
       <c r="R3" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="S3" s="141"/>
+      <c r="S3" s="136"/>
       <c r="T3" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="V3" s="134"/>
-      <c r="W3" s="134"/>
-      <c r="X3" s="134"/>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U3" s="95"/>
+      <c r="V3" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="138"/>
+      <c r="AA3" s="138"/>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B4" s="70" t="s">
         <v>165</v>
       </c>
@@ -1792,21 +1814,24 @@
       <c r="L4" s="95"/>
       <c r="M4" s="96"/>
       <c r="N4" s="17"/>
-      <c r="O4" s="139"/>
+      <c r="O4" s="134"/>
       <c r="P4" s="38"/>
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
       <c r="T4" s="80"/>
-      <c r="V4" s="83" t="s">
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="Y4" s="83" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="84"/>
-      <c r="X4" s="85" t="s">
+      <c r="Z4" s="84"/>
+      <c r="AA4" s="85" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>2</v>
       </c>
@@ -1841,21 +1866,24 @@
       </c>
       <c r="M5" s="96"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="139"/>
+      <c r="O5" s="134"/>
       <c r="P5" s="38"/>
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="80"/>
-      <c r="V5" s="86" t="s">
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="80"/>
+      <c r="Y5" s="86" t="s">
         <v>260</v>
       </c>
-      <c r="W5" s="87"/>
-      <c r="X5" s="85" t="s">
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="85" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="6"/>
       <c r="D6" s="34"/>
@@ -1869,21 +1897,24 @@
       <c r="L6" s="80"/>
       <c r="M6" s="96"/>
       <c r="N6" s="17"/>
-      <c r="O6" s="139"/>
+      <c r="O6" s="134"/>
       <c r="P6" s="38"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
       <c r="S6" s="27"/>
       <c r="T6" s="80"/>
-      <c r="V6" s="83" t="s">
+      <c r="U6" s="80"/>
+      <c r="V6" s="80"/>
+      <c r="W6" s="80"/>
+      <c r="Y6" s="83" t="s">
         <v>163</v>
       </c>
-      <c r="W6" s="88"/>
-      <c r="X6" s="85" t="s">
+      <c r="Z6" s="88"/>
+      <c r="AA6" s="85" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -1918,17 +1949,20 @@
       </c>
       <c r="M7" s="96"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="139"/>
+      <c r="O7" s="134"/>
       <c r="P7" s="38"/>
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
       <c r="S7" s="27"/>
       <c r="T7" s="80"/>
-      <c r="V7" s="106"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="7"/>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U7" s="80"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="80"/>
+      <c r="Y7" s="106"/>
+      <c r="Z7" s="107"/>
+      <c r="AA7" s="7"/>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B8" s="38"/>
       <c r="C8" s="89"/>
       <c r="D8" s="90"/>
@@ -1942,17 +1976,20 @@
       <c r="L8" s="80"/>
       <c r="M8" s="96"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="139"/>
+      <c r="O8" s="134"/>
       <c r="P8" s="38"/>
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="80"/>
-      <c r="V8" s="106"/>
-      <c r="W8" s="107"/>
-      <c r="X8" s="7"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U8" s="80"/>
+      <c r="V8" s="80"/>
+      <c r="W8" s="80"/>
+      <c r="Y8" s="106"/>
+      <c r="Z8" s="107"/>
+      <c r="AA8" s="7"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B9" s="70" t="s">
         <v>9</v>
       </c>
@@ -1965,11 +2002,14 @@
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="74"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="107"/>
-      <c r="X9" s="7"/>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="74"/>
+      <c r="Y9" s="106"/>
+      <c r="Z9" s="107"/>
+      <c r="AA9" s="7"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B10" s="71" t="s">
         <v>11</v>
       </c>
@@ -1982,11 +2022,14 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="74"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="107"/>
-      <c r="X10" s="7"/>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="Y10" s="106"/>
+      <c r="Z10" s="107"/>
+      <c r="AA10" s="7"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -2023,11 +2066,14 @@
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
       <c r="T11" s="74"/>
-      <c r="V11" s="106"/>
-      <c r="W11" s="107"/>
-      <c r="X11" s="7"/>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U11" s="74"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="74"/>
+      <c r="Y11" s="106"/>
+      <c r="Z11" s="107"/>
+      <c r="AA11" s="7"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G12" s="15"/>
       <c r="I12" s="26"/>
       <c r="O12" s="107"/>
@@ -2035,8 +2081,11 @@
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
       <c r="T12" s="74"/>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
         <v>1.2</v>
       </c>
@@ -2082,8 +2131,11 @@
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
       <c r="T13" s="74"/>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U13" s="74"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="74"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G14" s="15"/>
       <c r="I14" s="25">
         <f>'Template Format ANALISIS I'!B253</f>
@@ -2110,8 +2162,11 @@
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="74"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U14" s="74"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="74"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G15" s="15"/>
       <c r="J15" s="25"/>
       <c r="K15" s="25" t="str">
@@ -2128,8 +2183,11 @@
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
       <c r="T15" s="74"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U15" s="74"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="74"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B16" s="71"/>
       <c r="C16" s="10"/>
       <c r="O16" s="107"/>
@@ -2137,8 +2195,11 @@
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
       <c r="T16" s="74"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U16" s="74"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="74"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
         <v>2</v>
       </c>
@@ -2180,13 +2241,16 @@
         <v>82500</v>
       </c>
       <c r="O17" s="107"/>
-      <c r="P17" s="142"/>
+      <c r="P17" s="137"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="107"/>
       <c r="S17" s="7"/>
       <c r="T17" s="74"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U17" s="74"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="74"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
       <c r="E18" s="14"/>
       <c r="F18" s="100"/>
       <c r="G18" s="15"/>
@@ -2211,7 +2275,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="E19" s="14"/>
       <c r="F19" s="100"/>
       <c r="G19" s="15"/>
@@ -2224,12 +2288,12 @@
         <v>8550</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="E20" s="14"/>
       <c r="F20" s="100"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
         <v>3</v>
       </c>
@@ -2271,7 +2335,7 @@
         <v>27500</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I22" s="25">
         <f>'Template Format ANALISIS I'!B10</f>
         <v>8.3000000000000001E-3</v>
@@ -2293,7 +2357,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
       <c r="K23" s="13" t="str">
         <f>'Template Format ANALISIS I'!D11</f>
         <v>B.U &amp; Kentungan (10%)</v>
@@ -2303,7 +2367,7 @@
         <v>2849.6000000000004</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B25" s="13">
         <v>4</v>
       </c>
@@ -2345,7 +2409,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
       <c r="F26" s="100"/>
       <c r="G26" s="15"/>
       <c r="I26" s="25">
@@ -2369,7 +2433,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I27" s="25">
         <f>'Template Format ANALISIS I'!B17</f>
         <v>1.2</v>
@@ -2391,7 +2455,7 @@
         <v>240000</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
       <c r="K28" s="13" t="str">
         <f>'Template Format ANALISIS I'!D18</f>
         <v>B.U &amp; Kentungan (10%)</v>
@@ -2401,7 +2465,7 @@
         <v>27420</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B30" s="13">
         <v>5</v>
       </c>
@@ -2443,7 +2507,7 @@
         <v>85800</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I31" s="39">
         <f>'Template Format ANALISIS I'!B22</f>
         <v>3.9E-2</v>
@@ -2465,7 +2529,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I32" s="39">
         <f>'Template Format ANALISIS I'!B23</f>
         <v>0.39</v>
@@ -15267,7 +15331,7 @@
         <v>13950.000000000002</v>
       </c>
     </row>
-    <row r="609" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="609" spans="2:27" x14ac:dyDescent="0.3">
       <c r="J609" s="25"/>
       <c r="K609" s="25" t="str">
         <f>'Template Format ANALISIS I'!D365</f>
@@ -15279,13 +15343,13 @@
         <v>27675</v>
       </c>
     </row>
-    <row r="610" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="610" spans="2:27" x14ac:dyDescent="0.3">
       <c r="J610" s="25"/>
       <c r="K610" s="25"/>
       <c r="L610" s="42"/>
       <c r="M610" s="44"/>
     </row>
-    <row r="611" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="611" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B611" s="71" t="s">
         <v>235</v>
       </c>
@@ -15297,7 +15361,7 @@
       <c r="L611" s="42"/>
       <c r="M611" s="44"/>
     </row>
-    <row r="612" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="612" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B612" s="38">
         <v>1</v>
       </c>
@@ -15339,11 +15403,11 @@
         <f>'Template Format ANALISIS I'!F326</f>
         <v>110000</v>
       </c>
-      <c r="V612" s="129"/>
-      <c r="W612" s="6"/>
-      <c r="X612" s="7"/>
-    </row>
-    <row r="613" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y612" s="129"/>
+      <c r="Z612" s="6"/>
+      <c r="AA612" s="7"/>
+    </row>
+    <row r="613" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B613" s="38"/>
       <c r="C613" s="32"/>
       <c r="D613" s="34"/>
@@ -15371,11 +15435,11 @@
         <f>'Template Format ANALISIS I'!F327</f>
         <v>5400</v>
       </c>
-      <c r="V613" s="106"/>
-      <c r="W613" s="107"/>
-      <c r="X613" s="7"/>
-    </row>
-    <row r="614" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y613" s="106"/>
+      <c r="Z613" s="107"/>
+      <c r="AA613" s="7"/>
+    </row>
+    <row r="614" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B614" s="38"/>
       <c r="C614" s="32"/>
       <c r="D614" s="34"/>
@@ -15403,11 +15467,11 @@
         <f>'Template Format ANALISIS I'!F328</f>
         <v>58500</v>
       </c>
-      <c r="V614" s="129"/>
-      <c r="W614" s="133"/>
-      <c r="X614" s="7"/>
-    </row>
-    <row r="615" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y614" s="129"/>
+      <c r="Z614" s="133"/>
+      <c r="AA614" s="7"/>
+    </row>
+    <row r="615" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B615" s="38"/>
       <c r="C615" s="32"/>
       <c r="D615" s="34"/>
@@ -15436,7 +15500,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="616" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="616" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B616" s="38"/>
       <c r="C616" s="32"/>
       <c r="D616" s="34"/>
@@ -15465,7 +15529,7 @@
         <v>330000</v>
       </c>
     </row>
-    <row r="617" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="617" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B617" s="38"/>
       <c r="C617" s="32"/>
       <c r="D617" s="34"/>
@@ -15494,7 +15558,7 @@
         <v>7199.9999999999991</v>
       </c>
     </row>
-    <row r="618" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="618" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B618" s="38"/>
       <c r="C618" s="32"/>
       <c r="D618" s="34"/>
@@ -15523,7 +15587,7 @@
         <v>13950.000000000002</v>
       </c>
     </row>
-    <row r="619" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="619" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B619" s="38"/>
       <c r="C619" s="32"/>
       <c r="D619" s="34"/>
@@ -15543,7 +15607,7 @@
         <v>53135</v>
       </c>
     </row>
-    <row r="620" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="620" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B620" s="38"/>
       <c r="C620" s="32"/>
       <c r="D620" s="34"/>
@@ -15557,7 +15621,7 @@
       <c r="L620" s="66"/>
       <c r="M620" s="73"/>
     </row>
-    <row r="621" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="621" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B621" s="38">
         <v>2</v>
       </c>
@@ -15600,7 +15664,7 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="622" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="622" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B622" s="38"/>
       <c r="C622" s="32"/>
       <c r="D622" s="34"/>
@@ -15629,7 +15693,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="623" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="623" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B623" s="38"/>
       <c r="C623" s="32"/>
       <c r="D623" s="34"/>
@@ -15658,7 +15722,7 @@
         <v>45500</v>
       </c>
     </row>
-    <row r="624" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="624" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B624" s="38"/>
       <c r="C624" s="32"/>
       <c r="D624" s="34"/>
@@ -33778,13 +33842,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="V2:X3"/>
+  <mergeCells count="7">
+    <mergeCell ref="Y2:AA3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="O2:T2"/>
+    <mergeCell ref="V2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>